<commit_message>
application prop file added
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johnraju.chinnam.SSTECH\IdeaProjects\BaseFrameWork\Base_Framework\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johnraju.chinnam.SSTECH\IdeaProjects\PLSIRemoteRepo\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A102268F-33E8-4515-8F18-D12C671525E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DD7CD3-4B9E-403C-B421-23060AEFC492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="94">
   <si>
     <t>Description</t>
   </si>
@@ -299,17 +299,26 @@
     <t>CreateNew</t>
   </si>
   <si>
-    <t>King of Prussia</t>
-  </si>
-  <si>
     <t>DEVCom</t>
+  </si>
+  <si>
+    <t>01-02-2023</t>
+  </si>
+  <si>
+    <t>testLogin</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>mayuri.chigope@sstech.us</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -352,6 +361,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="5">
@@ -408,7 +422,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -422,6 +436,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -709,7 +726,7 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" style="2" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="31.7109375" style="2" customWidth="1" collapsed="1"/>
@@ -717,7 +734,7 @@
     <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -728,7 +745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -739,7 +756,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -750,7 +767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -761,10 +778,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="B6" s="3"/>
     </row>
   </sheetData>
@@ -787,7 +804,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
@@ -802,7 +819,7 @@
     <col min="12" max="12" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="7" customFormat="1">
       <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
@@ -843,7 +860,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -902,7 +919,7 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
     <col min="2" max="3" width="19.5703125" customWidth="1"/>
@@ -911,7 +928,7 @@
     <col min="6" max="6" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -931,7 +948,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -964,151 +981,178 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77821D73-03CE-4B19-A8A0-8DB2062EDEA4}">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" customWidth="1"/>
-    <col min="11" max="11" width="19" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20" customWidth="1"/>
-    <col min="15" max="15" width="23.7109375" customWidth="1"/>
-    <col min="16" max="16" width="18.85546875" customWidth="1"/>
-    <col min="17" max="17" width="17.140625" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" customWidth="1"/>
+    <col min="1" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" customWidth="1"/>
+    <col min="7" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="14" max="14" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20" customWidth="1"/>
+    <col min="17" max="17" width="23.7109375" customWidth="1"/>
+    <col min="18" max="18" width="18.85546875" customWidth="1"/>
+    <col min="19" max="19" width="17.140625" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="9" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>87</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="P1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="Q1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="5">
-        <v>44949</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
         <v>53</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>54</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
         <v>89</v>
       </c>
-      <c r="G2" t="s">
-        <v>90</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>57</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>58</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>60</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>61</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>62</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D8" s="8"/>
+    <row r="3" spans="1:20">
+      <c r="A3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="F8" s="8"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{0CD76549-F259-4CEA-9486-2001162D654E}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{6BF114DB-1414-485F-8657-1C265E0E026B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1120,7 +1164,7 @@
       <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -1140,7 +1184,7 @@
     <col min="17" max="17" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="9" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>87</v>
       </c>
@@ -1196,7 +1240,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -1265,7 +1309,7 @@
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -1278,7 +1322,7 @@
     <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="10" t="s">
         <v>66</v>
       </c>
@@ -1319,7 +1363,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
Files added for Team Members
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johnraju.chinnam.SSTECH\IdeaProjects\PLSIRemoteRepo\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80DDC52-827B-4F09-92CF-B5C49CFD866A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9DD7D8-CC34-4922-BD33-B099BA885EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="New appointment" sheetId="3" r:id="rId2"/>
-    <sheet name="Reject-Accept app" sheetId="4" r:id="rId3"/>
-    <sheet name="ClientMedical" sheetId="5" r:id="rId4"/>
-    <sheet name="ClientNonMedical" sheetId="6" r:id="rId5"/>
-    <sheet name="ADD Interpreter" sheetId="7" r:id="rId6"/>
+    <sheet name="Finance-Admin" sheetId="8" r:id="rId2"/>
+    <sheet name="New appointment" sheetId="3" r:id="rId3"/>
+    <sheet name="Reject-Accept app" sheetId="4" r:id="rId4"/>
+    <sheet name="ClientMedical" sheetId="5" r:id="rId5"/>
+    <sheet name="ClientNonMedical" sheetId="6" r:id="rId6"/>
+    <sheet name="ADD Interpreter" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="101">
   <si>
     <t>Description</t>
   </si>
@@ -65,9 +66,6 @@
     <t>xyz</t>
   </si>
   <si>
-    <t>Email Address</t>
-  </si>
-  <si>
     <t>Appointment Date</t>
   </si>
   <si>
@@ -89,9 +87,6 @@
     <t>Building</t>
   </si>
   <si>
-    <t>Patient Name</t>
-  </si>
-  <si>
     <t>Requested Language</t>
   </si>
   <si>
@@ -107,15 +102,9 @@
     <t>Abramson Building</t>
   </si>
   <si>
-    <t>CS</t>
-  </si>
-  <si>
     <t>Harsha</t>
   </si>
   <si>
-    <t>spanish</t>
-  </si>
-  <si>
     <t>Department</t>
   </si>
   <si>
@@ -143,21 +132,6 @@
     <t>Spanish</t>
   </si>
   <si>
-    <t>"16:15:00"</t>
-  </si>
-  <si>
-    <t>"16:35:00"</t>
-  </si>
-  <si>
-    <t>"23-12-2022"</t>
-  </si>
-  <si>
-    <t>Testname</t>
-  </si>
-  <si>
-    <t>Ashwini.</t>
-  </si>
-  <si>
     <t>Appointment Start Time</t>
   </si>
   <si>
@@ -302,9 +276,6 @@
     <t>DEVCom</t>
   </si>
   <si>
-    <t>01-02-2023</t>
-  </si>
-  <si>
     <t>testLogin</t>
   </si>
   <si>
@@ -321,6 +292,48 @@
   </si>
   <si>
     <t>ClientsMedical</t>
+  </si>
+  <si>
+    <t>approveSinglePendingStatus</t>
+  </si>
+  <si>
+    <t>approveFinancialArchivePendingAppointment</t>
+  </si>
+  <si>
+    <t>approveFinancialArchiveMultiplePendingAppointment</t>
+  </si>
+  <si>
+    <t>sortingColumnsFinancialArchive</t>
+  </si>
+  <si>
+    <t>07-02-2023</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>ClientsnonMedical</t>
+  </si>
+  <si>
+    <t>addScheduleAppointment</t>
+  </si>
+  <si>
+    <t>06-02-2023</t>
+  </si>
+  <si>
+    <t>04:00PM</t>
+  </si>
+  <si>
+    <t>05:00PM</t>
+  </si>
+  <si>
+    <t>DES_99</t>
+  </si>
+  <si>
+    <t>Sai</t>
+  </si>
+  <si>
+    <t>08-01-1998</t>
   </si>
 </sst>
 </file>
@@ -403,7 +416,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -426,19 +439,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -448,6 +473,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -806,121 +845,227 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D46A24-3205-4CDB-80C0-67C7443BF381}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D31F42-B4A6-433A-86B0-A7DD37BBCE9B}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="68.140625" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{82D8F002-3220-461F-86E5-D6CBF113B776}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{7DC562F3-6297-4C22-B964-1B2E0C56759A}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{23692AF0-1D1D-4CE2-8E4F-0737B8998945}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{C262461E-E34E-4071-94BC-437B89604088}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D46A24-3205-4CDB-80C0-67C7443BF381}">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" customWidth="1"/>
     <col min="10" max="10" width="11.85546875" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" customWidth="1"/>
     <col min="12" max="12" width="19.7109375" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:17" s="6" customFormat="1">
+      <c r="A1" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="I1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="K1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" s="7" t="s">
+      <c r="Q1" s="19"/>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="H2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="I2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="M2" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" t="s">
-        <v>41</v>
-      </c>
+      <c r="N2" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="O2" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{8C2EDEAB-5424-4075-9274-B543BBAA5DA1}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{21395195-EBF5-4024-8E8E-9D6B3DD35A35}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{953691FE-3F95-44A8-954A-65F42CFC5F53}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABF68EE-3805-47F6-94A7-65083586E1E3}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -939,22 +1084,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>33</v>
-      </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -965,16 +1110,16 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -988,12 +1133,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77821D73-03CE-4B19-A8A0-8DB2062EDEA4}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1017,191 +1162,254 @@
     <col min="20" max="20" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="9" customFormat="1">
-      <c r="A1" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:20" s="8" customFormat="1">
+      <c r="A1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="9" t="s">
+      <c r="O1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="T1" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>93</v>
+        <v>86</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>83</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>90</v>
+      <c r="D2" s="10" t="s">
+        <v>91</v>
       </c>
       <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="M2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="P2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
         <v>53</v>
       </c>
-      <c r="F2" t="s">
+      <c r="T2" t="s">
         <v>54</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>89</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="M2" t="s">
-        <v>57</v>
-      </c>
-      <c r="N2" t="s">
-        <v>58</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="P2" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>61</v>
-      </c>
-      <c r="R2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" t="s">
-        <v>62</v>
-      </c>
-      <c r="T2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>95</v>
+      <c r="D3" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
       <c r="K3" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:20">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="P5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>52</v>
+      </c>
+      <c r="R5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" t="s">
+        <v>53</v>
+      </c>
+      <c r="T5" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="8" spans="1:20">
-      <c r="F8" s="8"/>
+      <c r="F8" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{0CD76549-F259-4CEA-9486-2001162D654E}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{6BF114DB-1414-485F-8657-1C265E0E026B}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{83A3E713-7EB2-44BE-A455-FF627F946B25}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{121C4834-83C2-4F23-AF6A-A8C9AC582FEE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB8B0329-7A1D-489A-A07E-31F06CFF16B2}">
   <dimension ref="A1:R2"/>
   <sheetViews>
@@ -1229,116 +1437,116 @@
     <col min="17" max="17" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="9" customFormat="1">
-      <c r="A1" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="9" t="s">
+    <row r="1" spans="1:18" s="8" customFormat="1">
+      <c r="A1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="R1" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>86</v>
+        <v>79</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" t="s">
         <v>53</v>
       </c>
-      <c r="D2" t="s">
+      <c r="R2" t="s">
         <v>54</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>56</v>
-      </c>
-      <c r="J2" t="s">
-        <v>64</v>
-      </c>
-      <c r="K2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L2" t="s">
-        <v>58</v>
-      </c>
-      <c r="M2" t="s">
-        <v>59</v>
-      </c>
-      <c r="N2" t="s">
-        <v>60</v>
-      </c>
-      <c r="O2" t="s">
-        <v>61</v>
-      </c>
-      <c r="P2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1346,7 +1554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB21362-C935-4D70-8A2D-2CFAFF7C4674}">
   <dimension ref="A1:M2"/>
   <sheetViews>
@@ -1368,58 +1576,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="L1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E2">
         <v>8452</v>
@@ -1428,25 +1636,25 @@
         <v>9133221196</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="H2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="J2">
         <v>50081</v>
       </c>
       <c r="K2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New files for others and new methods added
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johnraju.chinnam.SSTECH\IdeaProjects\PLSIRemoteRepo\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9DD7D8-CC34-4922-BD33-B099BA885EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F4929B-EF4F-4552-BD7D-A29041AD5894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="ClientMedical" sheetId="5" r:id="rId5"/>
     <sheet name="ClientNonMedical" sheetId="6" r:id="rId6"/>
     <sheet name="ADD Interpreter" sheetId="7" r:id="rId7"/>
+    <sheet name="Interpreter_Offer" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="119">
   <si>
     <t>Description</t>
   </si>
@@ -102,9 +103,6 @@
     <t>Abramson Building</t>
   </si>
   <si>
-    <t>Harsha</t>
-  </si>
-  <si>
     <t>Department</t>
   </si>
   <si>
@@ -123,12 +121,6 @@
     <t>Interpreter Name</t>
   </si>
   <si>
-    <t>Matt Laborde</t>
-  </si>
-  <si>
-    <t>matt.laborde@sstech.us</t>
-  </si>
-  <si>
     <t>Spanish</t>
   </si>
   <si>
@@ -318,9 +310,6 @@
     <t>addScheduleAppointment</t>
   </si>
   <si>
-    <t>06-02-2023</t>
-  </si>
-  <si>
     <t>04:00PM</t>
   </si>
   <si>
@@ -330,17 +319,83 @@
     <t>DES_99</t>
   </si>
   <si>
-    <t>Sai</t>
-  </si>
-  <si>
     <t>08-01-1998</t>
+  </si>
+  <si>
+    <t>deepa.pattar@sstech.us</t>
+  </si>
+  <si>
+    <t>editPreference</t>
+  </si>
+  <si>
+    <t>makeAnOfferToInterpreter</t>
+  </si>
+  <si>
+    <t>acceptOfferByInterpreter</t>
+  </si>
+  <si>
+    <t>rescindOfferedToInterpreter</t>
+  </si>
+  <si>
+    <t>Appointment Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Request Reimbursement? </t>
+  </si>
+  <si>
+    <t>rejectAppointment</t>
+  </si>
+  <si>
+    <t>Telugu</t>
+  </si>
+  <si>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>acceptAppointment</t>
+  </si>
+  <si>
+    <t>returnAppointment</t>
+  </si>
+  <si>
+    <t>Confirmed</t>
+  </si>
+  <si>
+    <t>checkInAppointment</t>
+  </si>
+  <si>
+    <t>checkOutAndFinaliseAppointment</t>
+  </si>
+  <si>
+    <t>viewFinancialBreakdown</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>reshma.pokharkar@sstech.us</t>
+  </si>
+  <si>
+    <t>Resham Pokharkar</t>
+  </si>
+  <si>
+    <t>08-02-2023</t>
+  </si>
+  <si>
+    <t>Automation_SV</t>
+  </si>
+  <si>
+    <t>Tester</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -389,8 +444,17 @@
       <color rgb="FF6A8759"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF344767"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,6 +476,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,7 +527,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -487,6 +557,12 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -862,10 +938,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
@@ -876,7 +952,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>2</v>
@@ -887,7 +963,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -898,7 +974,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>2</v>
@@ -909,7 +985,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>2</v>
@@ -933,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D46A24-3205-4CDB-80C0-67C7443BF381}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -951,15 +1027,18 @@
     <col min="10" max="10" width="11.85546875" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" customWidth="1"/>
     <col min="12" max="12" width="19.7109375" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" customWidth="1"/>
     <col min="16" max="16" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="6" customFormat="1">
       <c r="A1" s="20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>1</v>
@@ -986,19 +1065,19 @@
         <v>17</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L1" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="O1" s="18" t="s">
         <v>36</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>39</v>
       </c>
       <c r="P1" s="15" t="s">
         <v>18</v>
@@ -1007,7 +1086,7 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>2</v>
@@ -1016,13 +1095,13 @@
         <v>3</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="E2" s="22" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F2" s="22" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G2" s="21" t="s">
         <v>19</v>
@@ -1037,22 +1116,22 @@
         <v>22</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>23</v>
+        <v>117</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="O2" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="P2" s="21" t="s">
-        <v>32</v>
+        <v>95</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>104</v>
       </c>
       <c r="Q2" s="13"/>
     </row>
@@ -1067,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABF68EE-3805-47F6-94A7-65083586E1E3}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1080,56 +1159,218 @@
     <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="19.140625" customWidth="1"/>
     <col min="6" max="6" width="24.42578125" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" s="24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="4" t="s">
+      <c r="H1" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
+      <c r="C2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{8DE6CF77-302C-4326-9EAE-3519D8EDFCBC}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{6FBA8F93-ABF4-456C-B097-2689B3FB54FD}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{74011E44-4203-4BC9-9098-395AA79CB576}"/>
-    <hyperlink ref="D2" r:id="rId4" xr:uid="{4F79843C-FD5E-401F-8C70-1D1E8E702262}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1164,10 +1405,10 @@
   <sheetData>
     <row r="1" spans="1:20" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
@@ -1176,10 +1417,10 @@
         <v>11</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>14</v>
@@ -1188,60 +1429,60 @@
         <v>15</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>17</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="Q1" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="R1" s="8" t="s">
         <v>18</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
@@ -1250,45 +1491,45 @@
         <v>20</v>
       </c>
       <c r="I2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J2" t="s">
         <v>22</v>
       </c>
       <c r="K2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="M2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="P2" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="Q2" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" t="s">
         <v>51</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>52</v>
-      </c>
-      <c r="R2" t="s">
-        <v>32</v>
-      </c>
-      <c r="S2" t="s">
-        <v>53</v>
-      </c>
-      <c r="T2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -1297,13 +1538,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
@@ -1312,18 +1553,18 @@
         <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J3" t="s">
         <v>22</v>
       </c>
       <c r="K3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>2</v>
@@ -1334,22 +1575,22 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G5" t="s">
         <v>19</v>
@@ -1358,40 +1599,40 @@
         <v>20</v>
       </c>
       <c r="I5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J5" t="s">
         <v>22</v>
       </c>
       <c r="K5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="M5" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="P5" t="s">
         <v>48</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="Q5" t="s">
         <v>49</v>
       </c>
-      <c r="O5" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="R5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" t="s">
+        <v>50</v>
+      </c>
+      <c r="T5" t="s">
         <v>51</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>52</v>
-      </c>
-      <c r="R5" t="s">
-        <v>32</v>
-      </c>
-      <c r="S5" t="s">
-        <v>53</v>
-      </c>
-      <c r="T5" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -1439,16 +1680,16 @@
   <sheetData>
     <row r="1" spans="1:18" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>14</v>
@@ -1457,54 +1698,54 @@
         <v>15</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>17</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>38</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="P1" s="8" t="s">
         <v>18</v>
       </c>
       <c r="Q1" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="R1" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -1513,40 +1754,40 @@
         <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
         <v>22</v>
       </c>
       <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" t="s">
         <v>47</v>
       </c>
-      <c r="J2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" t="s">
         <v>49</v>
       </c>
-      <c r="M2" t="s">
+      <c r="P2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" t="s">
         <v>50</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>51</v>
-      </c>
-      <c r="O2" t="s">
-        <v>52</v>
-      </c>
-      <c r="P2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>53</v>
-      </c>
-      <c r="R2" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1558,7 +1799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB21362-C935-4D70-8A2D-2CFAFF7C4674}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
@@ -1577,57 +1818,57 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>64</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E2">
         <v>8452</v>
@@ -1636,25 +1877,25 @@
         <v>9133221196</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J2">
         <v>50081</v>
       </c>
       <c r="K2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1665,4 +1906,91 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC50B798-C00F-4686-80C0-D4DC574A8857}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="13"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{C4A936E2-F158-4B3B-AAC9-BA2AA68BA3C6}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{01BBCDF9-6BF7-4C34-9C79-D6A2C2C9D47B}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{20410DF4-6485-4074-AC89-A128C9689C7F}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{06559F18-5AF5-4AA3-AB3B-2661BDBB0BFC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Module dependency removed and new tc added
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johnraju.chinnam.SSTECH\IdeaProjects\PLSIRemoteRepo\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DCF7A5A-4C35-4D95-90A1-2B3477B8480F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B803853-0B79-4243-98EC-D38B364F64BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
-    <sheet name="Finance-Admin" sheetId="8" r:id="rId2"/>
-    <sheet name="New appointment" sheetId="3" r:id="rId3"/>
+    <sheet name="New appointment" sheetId="3" r:id="rId2"/>
+    <sheet name="Finance-Admin" sheetId="8" r:id="rId3"/>
     <sheet name="Reject-Accept app" sheetId="4" r:id="rId4"/>
     <sheet name="ClientMedical" sheetId="5" r:id="rId5"/>
     <sheet name="ADD Interpreter" sheetId="7" r:id="rId6"/>
@@ -23,7 +23,6 @@
     <sheet name="Finance_Payout" sheetId="10" r:id="rId8"/>
     <sheet name="InterpreterAptTab" sheetId="11" r:id="rId9"/>
     <sheet name="Interpreter_Details" sheetId="12" r:id="rId10"/>
-    <sheet name="Inter_Lang Proficiency" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="200">
   <si>
     <t>Password</t>
   </si>
@@ -256,9 +255,6 @@
     <t>ClientsnonMedical</t>
   </si>
   <si>
-    <t>addScheduleAppointment</t>
-  </si>
-  <si>
     <t>04:00PM</t>
   </si>
   <si>
@@ -427,9 +423,6 @@
     <t>Complete</t>
   </si>
   <si>
-    <t>createNonMedicalAppointment</t>
-  </si>
-  <si>
     <t>SAT66</t>
   </si>
   <si>
@@ -568,9 +561,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>update_Interpreter_Availablity</t>
-  </si>
-  <si>
     <t>09:00AM</t>
   </si>
   <si>
@@ -616,26 +606,41 @@
     <t>Finance_Payout</t>
   </si>
   <si>
+    <t>scheduleAppointmentMedicalTest</t>
+  </si>
+  <si>
+    <t>createNonMedicalAppointmentTest</t>
+  </si>
+  <si>
+    <t>approveFinancialReviewPendingAppointment</t>
+  </si>
+  <si>
+    <t>Interpreter_Details</t>
+  </si>
+  <si>
+    <t>InterpreterName</t>
+  </si>
+  <si>
+    <t>Anirudh Roy</t>
+  </si>
+  <si>
     <t>InterpreterAptTab</t>
   </si>
   <si>
-    <t>Inter_Lang Proficiency</t>
-  </si>
-  <si>
-    <t>scheduleAppointmentMedicalTest</t>
-  </si>
-  <si>
-    <t>createNonMedicalAppointmentTest</t>
-  </si>
-  <si>
-    <t>approveFinancialReviewPendingAppointment</t>
+    <t>cancelNewAppointment</t>
+  </si>
+  <si>
+    <t>create_Interpreter_Availability</t>
+  </si>
+  <si>
+    <t>update_Interpreter_Availability</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -728,8 +733,14 @@
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF008000"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -760,8 +771,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -797,12 +814,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -882,13 +910,44 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1172,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1188,269 +1247,333 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="58" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="58" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="58" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="61" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="61" t="s">
+        <v>191</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="41" t="s">
-        <v>165</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" s="63" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="59" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="41" t="s">
-        <v>168</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="41" t="s">
-        <v>169</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="51" t="s">
-        <v>195</v>
-      </c>
-      <c r="B9" s="2" t="s">
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="51" t="s">
-        <v>196</v>
-      </c>
-      <c r="B11" s="2" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" s="59" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="B12" s="2" t="s">
+    <row r="24" spans="1:2">
+      <c r="A24" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="B13" s="2" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" s="64" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="2" t="s">
+    <row r="26" spans="1:2">
+      <c r="A26" s="64" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" s="2" t="s">
+    <row r="27" spans="1:2">
+      <c r="A27" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="38" t="s">
-        <v>177</v>
+      <c r="A28" s="62" t="s">
+        <v>199</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="38" t="s">
-        <v>181</v>
+      <c r="A29" s="62" t="s">
+        <v>178</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="38" t="s">
-        <v>172</v>
+      <c r="A30" s="62" t="s">
+        <v>170</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="30" t="s">
-        <v>173</v>
+      <c r="A31" s="61" t="s">
+        <v>198</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="38" t="s">
-        <v>172</v>
+      <c r="A32" s="60" t="s">
+        <v>171</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="30" t="s">
-        <v>173</v>
+      <c r="A33" s="65" t="s">
+        <v>109</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="65" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="65" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="65" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="30">
+      <c r="A37" s="65" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="30">
+      <c r="A38" s="65" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="65" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="60" t="s">
+        <v>197</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="66" t="s">
+        <v>192</v>
+      </c>
+      <c r="B41" s="54" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1461,15 +1584,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A5A638-D2C1-4C1E-8813-829FE21BCADA}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A2:A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="44.28515625" customWidth="1"/>
     <col min="2" max="2" width="29.5703125" customWidth="1"/>
     <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
@@ -1478,9 +1601,10 @@
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="37" t="s">
         <v>61</v>
       </c>
@@ -1491,138 +1615,185 @@
         <v>0</v>
       </c>
       <c r="D1" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="G1" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" s="52" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="E2" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="G1" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="H1" s="37" t="s">
+      <c r="F2" s="39" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="38" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="I3" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="B4" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="I4" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="J4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="30" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="38" t="s">
+      <c r="B5" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="G5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F6" t="s">
         <v>177</v>
       </c>
-      <c r="B2" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>178</v>
-      </c>
-      <c r="E2" s="39" t="s">
-        <v>179</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="H2" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="I2" s="30" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="H3" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="I3" s="30" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="38" t="s">
-        <v>172</v>
-      </c>
-      <c r="B4" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E4" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="50" t="s">
-        <v>183</v>
-      </c>
-      <c r="I4" s="50" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="B5" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="F5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="G5" t="s">
-        <v>136</v>
-      </c>
-      <c r="H5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>136</v>
+      <c r="G6" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" t="s">
+        <v>134</v>
+      </c>
+      <c r="I6" t="s">
+        <v>134</v>
+      </c>
+      <c r="J6" s="30" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1633,100 +1804,372 @@
     <hyperlink ref="C5" r:id="rId4" xr:uid="{2DAEEDB2-7E3F-429B-B695-7AB994FE65C5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F75AAA-D52E-4AD3-A677-ED328D0E323D}">
-  <dimension ref="A1:G3"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D46A24-3205-4CDB-80C0-67C7443BF381}">
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" style="12" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="24.42578125" customWidth="1"/>
+    <col min="18" max="18" width="13" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:19" s="6" customFormat="1">
       <c r="A1" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="P1" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="F1" s="37" t="s">
-        <v>171</v>
-      </c>
-      <c r="G1" s="30"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="38" t="s">
-        <v>172</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="49">
-        <v>10</v>
-      </c>
-      <c r="F2" s="49">
+      <c r="S1" s="32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="51" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="31"/>
+      <c r="E2" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" s="38" t="s">
+        <v>94</v>
+      </c>
+      <c r="O2" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="G2" s="30"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="P2" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q2" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="R2" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="S2" s="30"/>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="30"/>
+        <v>97</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>128</v>
+      </c>
       <c r="E3" s="30"/>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="N4" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="O4" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="P4" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q4" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="R4" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="S4" s="30"/>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="G5" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="K5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="M5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="N5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="O5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="P5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="R5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="S5" s="30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="5">
+        <v>44965</v>
+      </c>
+      <c r="F6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" t="s">
+        <v>75</v>
+      </c>
+      <c r="N6" t="s">
+        <v>94</v>
+      </c>
+      <c r="O6" t="s">
+        <v>95</v>
+      </c>
+      <c r="P6" s="5">
+        <v>35803</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>84</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{FC3A9483-3E95-47F0-8BD6-040F990E97C5}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{94A26A0D-7607-401F-93E7-39191CF9F859}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{953691FE-3F95-44A8-954A-65F42CFC5F53}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{E20E2CF2-F7CA-4630-B78A-96AFAF5BCC79}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{DA97C0E4-C8BB-4B1B-9A72-CEB76572843E}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{A19147BA-3A11-43A7-99EA-1DADEB7FAC25}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{DD59116B-88BF-4E41-8040-203ED37474F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D31F42-B4A6-433A-86B0-A7DD37BBCE9B}">
-  <dimension ref="A1:AD8"/>
+  <dimension ref="A1:AD9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1761,86 +2204,86 @@
         <v>0</v>
       </c>
       <c r="D1" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" s="33" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="G1" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="H1" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="I1" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="J1" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="K1" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="L1" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="M1" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="N1" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="O1" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="N1" s="40" t="s">
+      <c r="P1" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="O1" s="40" t="s">
+      <c r="Q1" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="R1" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="Q1" s="40" t="s">
+      <c r="S1" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="R1" s="40" t="s">
+      <c r="T1" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="S1" s="40" t="s">
+      <c r="U1" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="T1" s="40" t="s">
+      <c r="V1" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="U1" s="40" t="s">
+      <c r="W1" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="V1" s="40" t="s">
+      <c r="X1" s="40" t="s">
         <v>158</v>
       </c>
-      <c r="W1" s="40" t="s">
+      <c r="Y1" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="X1" s="40" t="s">
+      <c r="Z1" s="40" t="s">
         <v>160</v>
       </c>
-      <c r="Y1" s="40" t="s">
+      <c r="AA1" s="40" t="s">
         <v>161</v>
       </c>
-      <c r="Z1" s="40" t="s">
+      <c r="AB1" s="40" t="s">
         <v>162</v>
-      </c>
-      <c r="AA1" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="AB1" s="40" t="s">
-        <v>164</v>
       </c>
       <c r="AC1" s="30"/>
       <c r="AD1" s="30"/>
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="41" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>1</v>
@@ -1858,7 +2301,7 @@
         <v>2.65</v>
       </c>
       <c r="G2" s="44" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H2" s="45">
         <v>1</v>
@@ -1894,7 +2337,7 @@
         <v>20</v>
       </c>
       <c r="S2" s="46" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="T2" s="45">
         <v>1.25</v>
@@ -1924,7 +2367,7 @@
     </row>
     <row r="3" spans="1:30">
       <c r="A3" s="41" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>1</v>
@@ -1942,7 +2385,7 @@
         <v>2.65</v>
       </c>
       <c r="G3" s="44" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H3" s="45">
         <v>1</v>
@@ -1978,7 +2421,7 @@
         <v>20</v>
       </c>
       <c r="S3" s="46" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="T3" s="45">
         <v>1.25</v>
@@ -2122,7 +2565,7 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="41" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B7" s="34" t="s">
         <v>1</v>
@@ -2131,7 +2574,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
@@ -2162,7 +2605,7 @@
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="41" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B8" s="34" t="s">
         <v>1</v>
@@ -2170,6 +2613,44 @@
       <c r="C8" s="31" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="9" spans="1:30">
+      <c r="A9" s="57" t="s">
+        <v>192</v>
+      </c>
+      <c r="B9" s="56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="53"/>
+      <c r="O9" s="53"/>
+      <c r="P9" s="53"/>
+      <c r="Q9" s="53"/>
+      <c r="R9" s="53"/>
+      <c r="S9" s="53"/>
+      <c r="T9" s="53"/>
+      <c r="U9" s="53"/>
+      <c r="V9" s="53"/>
+      <c r="W9" s="53"/>
+      <c r="X9" s="53"/>
+      <c r="Y9" s="53"/>
+      <c r="Z9" s="53"/>
+      <c r="AA9" s="53"/>
+      <c r="AB9" s="53"/>
+      <c r="AC9" s="53"/>
+      <c r="AD9" s="53"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2180,309 +2661,10 @@
     <hyperlink ref="C3" r:id="rId5" xr:uid="{3FD6D116-216A-4423-835A-F97000FF95CC}"/>
     <hyperlink ref="C7" r:id="rId6" xr:uid="{E7BB4DFE-A00A-494B-B573-2FA848FA84CF}"/>
     <hyperlink ref="C8" r:id="rId7" xr:uid="{AADD8828-4D21-4908-9221-0DCFA4071DA4}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{955CE591-5FA8-44FA-B59E-9CF12EC2B812}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId8"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D46A24-3205-4CDB-80C0-67C7443BF381}">
-  <dimension ref="A1:S5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" customWidth="1"/>
-    <col min="14" max="14" width="22.140625" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" customWidth="1"/>
-    <col min="17" max="17" width="17.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" s="6" customFormat="1">
-      <c r="A1" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>83</v>
-      </c>
-      <c r="E1" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="32" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="O1" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="P1" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q1" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="R1" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="S1" s="32" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="39" t="s">
-        <v>127</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="L2" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="N2" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="O2" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="P2" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q2" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="R2" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="S2" s="30"/>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="E4" s="39" t="s">
-        <v>97</v>
-      </c>
-      <c r="F4" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="H4" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="N4" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="O4" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="P4" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q4" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="R4" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="S4" s="30"/>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="F5" s="39" t="s">
-        <v>137</v>
-      </c>
-      <c r="G5" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="H5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="J5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="K5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="L5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="M5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="N5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="O5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="P5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="R5" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="S5" s="30" t="s">
-        <v>139</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{953691FE-3F95-44A8-954A-65F42CFC5F53}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{E20E2CF2-F7CA-4630-B78A-96AFAF5BCC79}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{DA97C0E4-C8BB-4B1B-9A72-CEB76572843E}"/>
-    <hyperlink ref="C5" r:id="rId4" xr:uid="{A19147BA-3A11-43A7-99EA-1DADEB7FAC25}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -2490,8 +2672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABF68EE-3805-47F6-94A7-65083586E1E3}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2530,38 +2712,38 @@
         <v>10</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="J1" s="17"/>
       <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>85</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>86</v>
       </c>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
@@ -2569,7 +2751,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>1</v>
@@ -2578,19 +2760,19 @@
         <v>2</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>2</v>
       </c>
       <c r="G3" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>85</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>86</v>
       </c>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
@@ -2598,28 +2780,28 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>88</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>89</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
@@ -2627,7 +2809,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>1</v>
@@ -2636,19 +2818,19 @@
         <v>2</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
@@ -2656,7 +2838,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>1</v>
@@ -2665,50 +2847,50 @@
         <v>2</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>2</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>92</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>93</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
@@ -2729,7 +2911,7 @@
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3070,7 +3252,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3093,7 +3275,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>1</v>
@@ -3104,10 +3286,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -3115,7 +3297,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>1</v>
@@ -3126,7 +3308,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>1</v>
@@ -3180,61 +3362,61 @@
         <v>0</v>
       </c>
       <c r="D1" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>99</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" s="22" t="s">
         <v>102</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="22" t="s">
+      <c r="E3" s="22" t="s">
         <v>105</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="22" t="s">
+      <c r="E4" s="22" t="s">
         <v>108</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -3252,7 +3434,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3277,46 +3459,46 @@
         <v>17</v>
       </c>
       <c r="D1" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="H1" s="26" t="s">
         <v>123</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="24" t="s">
+      <c r="E2" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="29" t="s">
         <v>111</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>112</v>
       </c>
       <c r="G2" s="24"/>
       <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>1</v>
@@ -3325,10 +3507,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
@@ -3336,19 +3518,19 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>114</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>115</v>
       </c>
       <c r="F4" s="24"/>
       <c r="G4" s="24"/>
@@ -3356,7 +3538,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>1</v>
@@ -3365,10 +3547,10 @@
         <v>2</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F5" s="24"/>
       <c r="G5" s="24"/>
@@ -3376,7 +3558,7 @@
     </row>
     <row r="6" spans="1:8" ht="30">
       <c r="A6" s="28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>1</v>
@@ -3385,10 +3567,10 @@
         <v>2</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
@@ -3396,7 +3578,7 @@
     </row>
     <row r="7" spans="1:8" ht="30">
       <c r="A7" s="28" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>1</v>
@@ -3405,10 +3587,10 @@
         <v>2</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
@@ -3416,7 +3598,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B8" s="24" t="s">
         <v>1</v>
@@ -3425,16 +3607,16 @@
         <v>2</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H8" s="24"/>
     </row>

</xml_diff>

<commit_message>
Driver initialization code changed
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johnraju.chinnam.SSTECH\IdeaProjects\PLSIRemoteRepo\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B204CD3E-AB35-4C36-A990-EC13748A2C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0479DA6C-0759-4FAE-ABF8-DCD70601B0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
@@ -1234,7 +1234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -1586,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A5A638-D2C1-4C1E-8813-829FE21BCADA}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1720,7 +1720,7 @@
         <v>133</v>
       </c>
       <c r="G4" s="39" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="H4" s="49" t="s">
         <v>179</v>
@@ -1752,7 +1752,7 @@
         <v>133</v>
       </c>
       <c r="G5" t="s">
-        <v>133</v>
+        <v>39</v>
       </c>
       <c r="H5" s="30" t="s">
         <v>133</v>

</xml_diff>

<commit_message>
Listener added for each test class
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johnraju.chinnam.SSTECH\IdeaProjects\PLSIRemoteRepo\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0479DA6C-0759-4FAE-ABF8-DCD70601B0A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7E3A43-7003-4EAB-A9C3-9A1EAEBBFB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="201">
   <si>
     <t>Password</t>
   </si>
@@ -214,9 +214,6 @@
   </si>
   <si>
     <t>627</t>
-  </si>
-  <si>
-    <t>"2023-01-18"</t>
   </si>
   <si>
     <t>Test</t>
@@ -1248,332 +1245,332 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="54" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="54" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="54" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="56" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="56" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="57" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="55" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="55" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="55" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="55" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="55" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="57" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="57" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="57" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="56" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="55" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="59" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="59" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="59" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="59" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="30">
       <c r="A36" s="59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="30">
       <c r="A37" s="59" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="59" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="60" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B40" s="53" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="67" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B41" s="53" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -1586,7 +1583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47A5A638-D2C1-4C1E-8813-829FE21BCADA}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1606,39 +1603,39 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="37" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="E1" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="F1" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="F1" s="37" t="s">
-        <v>173</v>
-      </c>
       <c r="G1" s="37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H1" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="I1" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="I1" s="37" t="s">
-        <v>168</v>
-      </c>
       <c r="J1" s="52" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="38" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>1</v>
@@ -1647,30 +1644,30 @@
         <v>2</v>
       </c>
       <c r="D2" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="E2" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="F2" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="F2" s="39" t="s">
-        <v>176</v>
-      </c>
       <c r="G2" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J2" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="38" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B3" s="47" t="s">
         <v>1</v>
@@ -1679,30 +1676,30 @@
         <v>2</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H3" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J3" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" s="47" t="s">
         <v>1</v>
@@ -1711,30 +1708,30 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G4" s="39" t="s">
         <v>39</v>
       </c>
       <c r="H4" s="49" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I4" s="49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B5" s="47" t="s">
         <v>1</v>
@@ -1743,30 +1740,30 @@
         <v>2</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G5" t="s">
         <v>39</v>
       </c>
       <c r="H5" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J5" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="50" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1775,25 +1772,25 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J6" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -1841,16 +1838,16 @@
   <sheetData>
     <row r="1" spans="1:19" s="6" customFormat="1">
       <c r="A1" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="33" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" s="32" t="s">
         <v>3</v>
@@ -1883,7 +1880,7 @@
         <v>26</v>
       </c>
       <c r="O1" s="35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P1" s="35" t="s">
         <v>27</v>
@@ -1892,15 +1889,15 @@
         <v>10</v>
       </c>
       <c r="R1" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="S1" s="32" t="s">
         <v>123</v>
-      </c>
-      <c r="S1" s="32" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="51" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>1</v>
@@ -1910,13 +1907,13 @@
       </c>
       <c r="D2" s="31"/>
       <c r="E2" s="39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F2" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="39" t="s">
         <v>72</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>73</v>
       </c>
       <c r="H2" s="38" t="s">
         <v>11</v>
@@ -1934,28 +1931,28 @@
         <v>34</v>
       </c>
       <c r="M2" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="N2" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="O2" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="P2" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="N2" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="O2" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="P2" s="39" t="s">
-        <v>75</v>
-      </c>
       <c r="Q2" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R2" s="30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S2" s="30"/>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>1</v>
@@ -1964,7 +1961,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="30"/>
@@ -1984,7 +1981,7 @@
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" s="34" t="s">
         <v>1</v>
@@ -1993,16 +1990,16 @@
         <v>2</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F4" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="39" t="s">
         <v>72</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>73</v>
       </c>
       <c r="H4" s="38" t="s">
         <v>11</v>
@@ -2020,28 +2017,28 @@
         <v>34</v>
       </c>
       <c r="M4" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="N4" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="N4" s="38" t="s">
+      <c r="O4" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="O4" s="38" t="s">
+      <c r="P4" s="39" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q4" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="R4" s="30" t="s">
         <v>130</v>
-      </c>
-      <c r="P4" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q4" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="R4" s="30" t="s">
-        <v>131</v>
       </c>
       <c r="S4" s="30"/>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>1</v>
@@ -2050,57 +2047,57 @@
         <v>2</v>
       </c>
       <c r="D5" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="E5" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="F5" s="39" t="s">
+      <c r="G5" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="G5" s="39" t="s">
+      <c r="H5" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="K5" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="M5" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="N5" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="O5" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="P5" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q5" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="R5" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="S5" s="30" t="s">
         <v>135</v>
-      </c>
-      <c r="H5" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="J5" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="K5" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="L5" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="M5" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="N5" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="O5" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="P5" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="Q5" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="R5" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="S5" s="30" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B6" s="31" t="s">
         <v>1</v>
@@ -2109,16 +2106,16 @@
         <v>2</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E6" s="5">
         <v>44965</v>
       </c>
       <c r="F6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" t="s">
         <v>72</v>
-      </c>
-      <c r="G6" t="s">
-        <v>73</v>
       </c>
       <c r="H6" t="s">
         <v>11</v>
@@ -2136,24 +2133,24 @@
         <v>34</v>
       </c>
       <c r="M6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N6" t="s">
+        <v>92</v>
+      </c>
+      <c r="O6" t="s">
         <v>93</v>
-      </c>
-      <c r="O6" t="s">
-        <v>94</v>
       </c>
       <c r="P6" s="5">
         <v>35803</v>
       </c>
       <c r="Q6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="64" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B7" s="63" t="s">
         <v>1</v>
@@ -2162,16 +2159,16 @@
         <v>2</v>
       </c>
       <c r="D7" s="61" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E7" s="66" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F7" s="66" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="66" t="s">
         <v>72</v>
-      </c>
-      <c r="G7" s="66" t="s">
-        <v>73</v>
       </c>
       <c r="H7" s="65" t="s">
         <v>11</v>
@@ -2189,22 +2186,22 @@
         <v>34</v>
       </c>
       <c r="M7" s="65" t="s">
+        <v>199</v>
+      </c>
+      <c r="N7" s="65" t="s">
         <v>200</v>
       </c>
-      <c r="N7" s="65" t="s">
-        <v>201</v>
-      </c>
       <c r="O7" s="65" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P7" s="66" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q7" s="61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R7" s="61" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S7" s="61"/>
     </row>
@@ -2253,95 +2250,95 @@
   <sheetData>
     <row r="1" spans="1:30">
       <c r="A1" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="33" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="F1" s="33" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="G1" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="I1" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="I1" s="40" t="s">
+      <c r="J1" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="K1" s="40" t="s">
         <v>143</v>
       </c>
-      <c r="K1" s="40" t="s">
+      <c r="L1" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="L1" s="40" t="s">
+      <c r="M1" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="N1" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="N1" s="40" t="s">
+      <c r="O1" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="O1" s="40" t="s">
+      <c r="P1" s="40" t="s">
         <v>148</v>
       </c>
-      <c r="P1" s="40" t="s">
+      <c r="Q1" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="Q1" s="40" t="s">
+      <c r="R1" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="R1" s="40" t="s">
+      <c r="S1" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="S1" s="40" t="s">
+      <c r="T1" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="T1" s="40" t="s">
+      <c r="U1" s="40" t="s">
         <v>153</v>
       </c>
-      <c r="U1" s="40" t="s">
+      <c r="V1" s="40" t="s">
         <v>154</v>
       </c>
-      <c r="V1" s="40" t="s">
+      <c r="W1" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="W1" s="40" t="s">
+      <c r="X1" s="40" t="s">
         <v>156</v>
       </c>
-      <c r="X1" s="40" t="s">
+      <c r="Y1" s="40" t="s">
         <v>157</v>
       </c>
-      <c r="Y1" s="40" t="s">
+      <c r="Z1" s="40" t="s">
         <v>158</v>
       </c>
-      <c r="Z1" s="40" t="s">
+      <c r="AA1" s="40" t="s">
         <v>159</v>
       </c>
-      <c r="AA1" s="40" t="s">
+      <c r="AB1" s="40" t="s">
         <v>160</v>
-      </c>
-      <c r="AB1" s="40" t="s">
-        <v>161</v>
       </c>
       <c r="AC1" s="30"/>
       <c r="AD1" s="30"/>
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="41" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>1</v>
@@ -2359,7 +2356,7 @@
         <v>2.65</v>
       </c>
       <c r="G2" s="44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H2" s="45">
         <v>1</v>
@@ -2395,7 +2392,7 @@
         <v>20</v>
       </c>
       <c r="S2" s="46" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="T2" s="45">
         <v>1.25</v>
@@ -2425,7 +2422,7 @@
     </row>
     <row r="3" spans="1:30">
       <c r="A3" s="41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>1</v>
@@ -2443,7 +2440,7 @@
         <v>2.65</v>
       </c>
       <c r="G3" s="44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H3" s="45">
         <v>1</v>
@@ -2479,7 +2476,7 @@
         <v>20</v>
       </c>
       <c r="S3" s="46" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="T3" s="45">
         <v>1.25</v>
@@ -2509,7 +2506,7 @@
     </row>
     <row r="4" spans="1:30">
       <c r="A4" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="34" t="s">
         <v>1</v>
@@ -2547,7 +2544,7 @@
     </row>
     <row r="5" spans="1:30">
       <c r="A5" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>1</v>
@@ -2585,7 +2582,7 @@
     </row>
     <row r="6" spans="1:30">
       <c r="A6" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="34" t="s">
         <v>1</v>
@@ -2623,7 +2620,7 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B7" s="34" t="s">
         <v>1</v>
@@ -2632,7 +2629,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
@@ -2663,7 +2660,7 @@
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="41" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B8" s="34" t="s">
         <v>1</v>
@@ -2710,7 +2707,7 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>16</v>
@@ -2731,38 +2728,38 @@
         <v>10</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J1" s="17"/>
       <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>83</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>84</v>
       </c>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
@@ -2770,7 +2767,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>1</v>
@@ -2779,19 +2776,19 @@
         <v>2</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>2</v>
       </c>
       <c r="G3" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="12" t="s">
         <v>83</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>84</v>
       </c>
       <c r="I3" s="12"/>
       <c r="J3" s="12"/>
@@ -2799,28 +2796,28 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>86</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>87</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="12"/>
@@ -2828,7 +2825,7 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>1</v>
@@ -2837,19 +2834,19 @@
         <v>2</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
@@ -2857,7 +2854,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>1</v>
@@ -2866,50 +2863,50 @@
         <v>2</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>2</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>90</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>91</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
@@ -2929,8 +2926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77821D73-03CE-4B19-A8A0-8DB2062EDEA4}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2956,10 +2953,10 @@
   <sheetData>
     <row r="1" spans="1:20" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>0</v>
@@ -2995,7 +2992,7 @@
         <v>26</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O1" s="8" t="s">
         <v>27</v>
@@ -3018,16 +3015,16 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
         <v>32</v>
@@ -3042,7 +3039,7 @@
         <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J2" t="s">
         <v>14</v>
@@ -3059,8 +3056,8 @@
       <c r="N2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>60</v>
+      <c r="O2" s="5">
+        <v>35082</v>
       </c>
       <c r="P2" t="s">
         <v>37</v>
@@ -3080,16 +3077,16 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
         <v>32</v>
@@ -3104,7 +3101,7 @@
         <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J3" t="s">
         <v>14</v>
@@ -3121,8 +3118,8 @@
       <c r="N3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="5" t="s">
-        <v>60</v>
+      <c r="O3" s="5">
+        <v>35813</v>
       </c>
       <c r="P3" t="s">
         <v>37</v>
@@ -3283,10 +3280,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>0</v>
@@ -3294,7 +3291,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>1</v>
@@ -3305,10 +3302,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -3316,7 +3313,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>1</v>
@@ -3327,7 +3324,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>1</v>
@@ -3372,70 +3369,70 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>97</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" s="22" t="s">
         <v>100</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="22" t="s">
+      <c r="E3" s="22" t="s">
         <v>103</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="22" t="s">
+      <c r="E4" s="22" t="s">
         <v>106</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3469,7 +3466,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>16</v>
@@ -3478,46 +3475,46 @@
         <v>17</v>
       </c>
       <c r="D1" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="H1" s="26" t="s">
         <v>121</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="24" t="s">
+      <c r="E2" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="F2" s="29" t="s">
         <v>109</v>
-      </c>
-      <c r="E2" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>110</v>
       </c>
       <c r="G2" s="24"/>
       <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" s="24" t="s">
         <v>1</v>
@@ -3526,10 +3523,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
@@ -3537,19 +3534,19 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>112</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>109</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>113</v>
       </c>
       <c r="F4" s="24"/>
       <c r="G4" s="24"/>
@@ -3557,7 +3554,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="28" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>1</v>
@@ -3566,10 +3563,10 @@
         <v>2</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F5" s="24"/>
       <c r="G5" s="24"/>
@@ -3577,7 +3574,7 @@
     </row>
     <row r="6" spans="1:8" ht="30">
       <c r="A6" s="28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>1</v>
@@ -3586,10 +3583,10 @@
         <v>2</v>
       </c>
       <c r="D6" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
@@ -3597,7 +3594,7 @@
     </row>
     <row r="7" spans="1:8" ht="30">
       <c r="A7" s="28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>1</v>
@@ -3606,10 +3603,10 @@
         <v>2</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F7" s="24"/>
       <c r="G7" s="24"/>
@@ -3617,7 +3614,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B8" s="24" t="s">
         <v>1</v>
@@ -3626,16 +3623,16 @@
         <v>2</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E8" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H8" s="24"/>
     </row>

</xml_diff>

<commit_message>
Added canselfbook TC added
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johnraju.chinnam.SSTECH\IdeaProjects\PLSIRemoteRepo\PLSIAutomationBase\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashwini.G\Desktop\PLSIAutomationBaseFramework\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7E3A43-7003-4EAB-A9C3-9A1EAEBBFB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1243482E-11F1-4361-A470-770B130642B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="202">
   <si>
     <t>Password</t>
   </si>
@@ -637,13 +637,16 @@
   </si>
   <si>
     <t>Vikrant S</t>
+  </si>
+  <si>
+    <t>selfBookAppointment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -741,6 +744,12 @@
       <sz val="10"/>
       <color rgb="FF008000"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1229,18 +1238,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="52.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="31.7109375" style="2" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="1" width="52.109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.6640625" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.33203125" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1">
@@ -1381,17 +1390,17 @@
         <v>184</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" s="53" customFormat="1">
       <c r="A18" s="55" t="s">
-        <v>64</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>185</v>
+        <v>201</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="55" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>185</v>
@@ -1399,15 +1408,15 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="55" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>186</v>
@@ -1415,7 +1424,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>186</v>
@@ -1423,7 +1432,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="55" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>186</v>
@@ -1431,15 +1440,15 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="55" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="55" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>187</v>
@@ -1447,23 +1456,23 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="55" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="57" t="s">
-        <v>197</v>
+      <c r="A27" s="55" t="s">
+        <v>104</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="57" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>191</v>
@@ -1471,39 +1480,39 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="57" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="56" t="s">
-        <v>196</v>
+      <c r="A30" s="57" t="s">
+        <v>168</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="55" t="s">
-        <v>169</v>
+      <c r="A31" s="56" t="s">
+        <v>196</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="59" t="s">
-        <v>107</v>
+      <c r="A32" s="55" t="s">
+        <v>169</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="59" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>194</v>
@@ -1511,7 +1520,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="59" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>194</v>
@@ -1519,57 +1528,65 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="59" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="30">
+    <row r="36" spans="1:2">
       <c r="A36" s="59" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="30">
+    <row r="37" spans="1:2" ht="28.8">
       <c r="A37" s="59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" ht="28.8">
       <c r="A38" s="59" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="55" t="s">
+      <c r="A39" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="55" t="s">
         <v>195</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="60" t="s">
+    <row r="41" spans="1:2">
+      <c r="A41" s="60" t="s">
         <v>190</v>
       </c>
-      <c r="B40" s="53" t="s">
+      <c r="B41" s="53" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="67" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" s="67" t="s">
         <v>198</v>
       </c>
-      <c r="B41" s="53" t="s">
+      <c r="B42" s="53" t="s">
         <v>183</v>
       </c>
     </row>
@@ -1587,18 +1604,18 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="44.28515625" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="1" max="1" width="44.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
-    <col min="6" max="6" width="38.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="26.88671875" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1813,27 +1830,27 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" customWidth="1"/>
-    <col min="14" max="14" width="22.140625" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" customWidth="1"/>
-    <col min="17" max="17" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="19.6640625" customWidth="1"/>
+    <col min="14" max="14" width="22.109375" customWidth="1"/>
+    <col min="15" max="15" width="15.88671875" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" customWidth="1"/>
+    <col min="17" max="17" width="24.44140625" customWidth="1"/>
     <col min="18" max="18" width="13" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" customWidth="1"/>
+    <col min="19" max="19" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="6" customFormat="1">
@@ -2227,25 +2244,25 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="68.140625" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" customWidth="1"/>
-    <col min="4" max="4" width="44.5703125" customWidth="1"/>
-    <col min="16" max="16" width="20.5703125" customWidth="1"/>
-    <col min="17" max="17" width="22.7109375" customWidth="1"/>
-    <col min="18" max="18" width="22.42578125" customWidth="1"/>
-    <col min="19" max="19" width="21.7109375" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" customWidth="1"/>
-    <col min="22" max="22" width="20.28515625" customWidth="1"/>
-    <col min="23" max="23" width="18.42578125" customWidth="1"/>
-    <col min="24" max="24" width="19.42578125" customWidth="1"/>
-    <col min="25" max="25" width="23.7109375" customWidth="1"/>
-    <col min="26" max="26" width="23.85546875" customWidth="1"/>
-    <col min="27" max="27" width="25.7109375" customWidth="1"/>
-    <col min="28" max="28" width="20.85546875" customWidth="1"/>
-    <col min="29" max="29" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="68.109375" customWidth="1"/>
+    <col min="2" max="2" width="42.88671875" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" customWidth="1"/>
+    <col min="4" max="4" width="44.5546875" customWidth="1"/>
+    <col min="16" max="16" width="20.5546875" customWidth="1"/>
+    <col min="17" max="17" width="22.6640625" customWidth="1"/>
+    <col min="18" max="18" width="22.44140625" customWidth="1"/>
+    <col min="19" max="19" width="21.6640625" customWidth="1"/>
+    <col min="20" max="20" width="15.6640625" customWidth="1"/>
+    <col min="22" max="22" width="20.33203125" customWidth="1"/>
+    <col min="23" max="23" width="18.44140625" customWidth="1"/>
+    <col min="24" max="24" width="19.44140625" customWidth="1"/>
+    <col min="25" max="25" width="23.6640625" customWidth="1"/>
+    <col min="26" max="26" width="23.88671875" customWidth="1"/>
+    <col min="27" max="27" width="25.6640625" customWidth="1"/>
+    <col min="28" max="28" width="20.88671875" customWidth="1"/>
+    <col min="29" max="29" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30">
@@ -2686,23 +2703,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABF68EE-3805-47F6-94A7-65083586E1E3}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="3" width="37.42578125" customWidth="1"/>
+    <col min="1" max="1" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="3" width="37.44140625" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -2912,13 +2929,43 @@
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
     </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="62" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{0D458867-A002-45E1-B365-545961492A16}"/>
     <hyperlink ref="E3:E7" r:id="rId2" display="deepa.pattar@sstech.us" xr:uid="{61492ADE-3336-44E6-9318-42D2D7523F4D}"/>
+    <hyperlink ref="C8" r:id="rId3" xr:uid="{F9541A1A-083A-467B-8FAB-8925956AA176}"/>
+    <hyperlink ref="E8" r:id="rId4" xr:uid="{7B6F783C-2668-461F-8AAE-3907A5CECDFB}"/>
+    <hyperlink ref="F8" r:id="rId5" xr:uid="{469E87F4-86D5-44DD-95F4-0B88A4123999}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -2926,29 +2973,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77821D73-03CE-4B19-A8A0-8DB2062EDEA4}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="3" width="24.42578125" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" customWidth="1"/>
-    <col min="7" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="1" max="3" width="24.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" customWidth="1"/>
+    <col min="7" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="19.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" customWidth="1"/>
     <col min="13" max="13" width="19" customWidth="1"/>
-    <col min="14" max="14" width="15.5703125" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5546875" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20" customWidth="1"/>
-    <col min="17" max="17" width="23.7109375" customWidth="1"/>
-    <col min="18" max="18" width="18.85546875" customWidth="1"/>
-    <col min="19" max="19" width="17.140625" customWidth="1"/>
-    <col min="20" max="20" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="23.6640625" customWidth="1"/>
+    <col min="18" max="18" width="18.88671875" customWidth="1"/>
+    <col min="19" max="19" width="17.109375" customWidth="1"/>
+    <col min="20" max="20" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="8" customFormat="1">
@@ -3158,17 +3205,17 @@
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -3271,11 +3318,11 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="1" max="1" width="33.88671875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="32.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3358,12 +3405,12 @@
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="36.140625" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="36.109375" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3453,15 +3500,15 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="49" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.44140625" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -3572,7 +3619,7 @@
       <c r="G5" s="24"/>
       <c r="H5" s="24"/>
     </row>
-    <row r="6" spans="1:8" ht="30">
+    <row r="6" spans="1:8" ht="28.8">
       <c r="A6" s="28" t="s">
         <v>114</v>
       </c>
@@ -3592,7 +3639,7 @@
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
     </row>
-    <row r="7" spans="1:8" ht="30">
+    <row r="7" spans="1:8" ht="28.8">
       <c r="A7" s="28" t="s">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
ack  click code added
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johnraju.chinnam.SSTECH\IdeaProjects\PLSIRemoteRepo\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426E07C7-370F-4F23-9C8E-B23E7D24E235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6C5405-61DA-4F66-832B-1B48120F0EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="204">
   <si>
     <t>Password</t>
   </si>
@@ -643,6 +643,9 @@
   </si>
   <si>
     <t>18-01-1998</t>
+  </si>
+  <si>
+    <t>mayuri.chigope@sstech.us</t>
   </si>
 </sst>
 </file>
@@ -2974,8 +2977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77821D73-03CE-4B19-A8A0-8DB2062EDEA4}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3066,7 +3069,7 @@
         <v>63</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>1</v>
+        <v>203</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -3128,7 +3131,7 @@
         <v>69</v>
       </c>
       <c r="B3" s="61" t="s">
-        <v>1</v>
+        <v>203</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
@@ -3192,9 +3195,11 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{6BF114DB-1414-485F-8657-1C265E0E026B}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{121C4834-83C2-4F23-AF6A-A8C9AC582FEE}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{80FD45D6-A75F-4B4E-BC27-073308CC3D38}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{FB3398BF-201E-4399-A6CE-9722D57CBCB8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed skipped scenarios and canself TC fix
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johnraju.chinnam.SSTECH\IdeaProjects\PLSIRemoteRepo\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEEEF82-8454-484D-A120-BF6166E08272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E111090-B75D-4888-AFA6-876DFD35716D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1244,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3517,7 +3517,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
logout added for add request, fix for add lang prof
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnraju.chinnam.SSTECH.000\IdeaProjects\PLSI_NewClone\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B729BDEC-3CCC-46E6-A4D1-461BB19BD093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98164DB0-E083-40F0-81F9-242A4356D539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
@@ -637,9 +637,6 @@
     <t>18-01-1998</t>
   </si>
   <si>
-    <t>mayuri.chigope@sstech.us</t>
-  </si>
-  <si>
     <t>requestClientsNonMedicalAppointment</t>
   </si>
   <si>
@@ -710,6 +707,9 @@
   </si>
   <si>
     <t>Kennedy</t>
+  </si>
+  <si>
+    <t>mayuri.chitgope@sstech.us</t>
   </si>
 </sst>
 </file>
@@ -1468,18 +1468,18 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="49" t="s">
+        <v>201</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>202</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="49" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1660,10 +1660,10 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="49" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1902,7 +1902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F3517F0-85DC-46BC-AE96-D76A2E9F5DE3}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1932,75 +1932,75 @@
         <v>0</v>
       </c>
       <c r="D1" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="F1" s="32" t="s">
         <v>208</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="G1" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="I1" s="32" t="s">
         <v>211</v>
       </c>
-      <c r="I1" s="32" t="s">
+      <c r="J1" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="K1" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="K1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="M1" s="32" t="s">
         <v>215</v>
-      </c>
-      <c r="M1" s="32" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="49" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>204</v>
       </c>
-      <c r="B2" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="60" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>205</v>
-      </c>
       <c r="E2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G2" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="60" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I2" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="J2" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="K2" t="s">
         <v>219</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>220</v>
       </c>
-      <c r="L2" t="s">
-        <v>221</v>
-      </c>
       <c r="M2" s="28" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3160,8 +3160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77821D73-03CE-4B19-A8A0-8DB2062EDEA4}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3250,10 +3250,10 @@
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="49" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -3312,10 +3312,10 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="49" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B3" s="61" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
@@ -3380,7 +3380,7 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{6BF114DB-1414-485F-8657-1C265E0E026B}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{121C4834-83C2-4F23-AF6A-A8C9AC582FEE}"/>
     <hyperlink ref="B2" r:id="rId3" xr:uid="{80FD45D6-A75F-4B4E-BC27-073308CC3D38}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{FB3398BF-201E-4399-A6CE-9722D57CBCB8}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{B32A490F-FAF2-470C-A8A8-88CF78E1A4A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>

</xml_diff>

<commit_message>
change the user Email id for login
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaiVamshi.Kotla.SSTECH\PLSIBaseFramework\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0382B91E-B16F-4F1E-A590-E06F3F593622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC96B2C2-104D-4633-8F9D-D14F12CF0A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="227">
   <si>
     <t>Password</t>
   </si>
@@ -713,6 +713,9 @@
   </si>
   <si>
     <t>gangadhar.m@sstech.us</t>
+  </si>
+  <si>
+    <t>sravani.bandaru@sstech.us</t>
   </si>
 </sst>
 </file>
@@ -909,7 +912,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1002,6 +1005,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1995,8 +2001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D46A24-3205-4CDB-80C0-67C7443BF381}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2084,8 +2090,8 @@
       <c r="A2" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>1</v>
+      <c r="B2" s="50" t="s">
+        <v>226</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -2138,8 +2144,8 @@
       <c r="A3" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>1</v>
+      <c r="B3" s="50" t="s">
+        <v>226</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
@@ -2152,8 +2158,8 @@
       <c r="A4" t="s">
         <v>185</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>1</v>
+      <c r="B4" s="50" t="s">
+        <v>226</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
@@ -2208,8 +2214,8 @@
       <c r="A5" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>1</v>
+      <c r="B5" s="50" t="s">
+        <v>226</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>2</v>
@@ -2267,8 +2273,8 @@
       <c r="A6" t="s">
         <v>190</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>1</v>
+      <c r="B6" s="50" t="s">
+        <v>226</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -2320,8 +2326,8 @@
       <c r="A7" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>1</v>
+      <c r="B7" s="50" t="s">
+        <v>226</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>2</v>
@@ -2378,11 +2384,12 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{E20E2CF2-F7CA-4630-B78A-96AFAF5BCC79}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{DA97C0E4-C8BB-4B1B-9A72-CEB76572843E}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{A19147BA-3A11-43A7-99EA-1DADEB7FAC25}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{DD59116B-88BF-4E41-8040-203ED37474F9}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{D5D17004-3FC0-4EA0-98DC-166C1EB3FCE4}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{D5D17004-3FC0-4EA0-98DC-166C1EB3FCE4}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{B7145825-7747-4E7F-882E-DC2FFB5E3E1F}"/>
+    <hyperlink ref="B3:B7" r:id="rId7" display="sravani.bandaru@sstech.us" xr:uid="{D85EA05C-8D3F-4BDF-8BAC-7AC8A1C3A7EC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -2746,7 +2753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ABF68EE-3805-47F6-94A7-65083586E1E3}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -3230,7 +3237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB21362-C935-4D70-8A2D-2CFAFF7C4674}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modify the url and user mail id to execute
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaiVamshi.Kotla.SSTECH\PLSIBaseFramework\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC96B2C2-104D-4633-8F9D-D14F12CF0A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817142F6-8EA1-4146-B7BF-9ACE9FC92CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="229">
   <si>
     <t>Password</t>
   </si>
@@ -716,6 +716,12 @@
   </si>
   <si>
     <t>sravani.bandaru@sstech.us</t>
+  </si>
+  <si>
+    <t>poojaanusha96@gmail.com</t>
+  </si>
+  <si>
+    <t>vineela.cherukuri@sstech.us</t>
   </si>
 </sst>
 </file>
@@ -912,7 +918,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -969,9 +975,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1293,7 +1296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="C27" workbookViewId="0">
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
@@ -1314,7 +1317,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>158</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1323,7 +1326,7 @@
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="39" t="s">
         <v>161</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1332,7 +1335,7 @@
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="40" t="s">
         <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1340,7 +1343,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="40" t="s">
         <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1348,7 +1351,7 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="40" t="s">
         <v>65</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1356,7 +1359,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="39" t="s">
         <v>162</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1364,7 +1367,7 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="41" t="s">
         <v>184</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1372,7 +1375,7 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="40" t="s">
         <v>92</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1380,7 +1383,7 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="41" t="s">
         <v>185</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1388,7 +1391,7 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="42" t="s">
         <v>128</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1396,7 +1399,7 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="40" t="s">
         <v>78</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1404,7 +1407,7 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="43" t="s">
         <v>81</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1412,7 +1415,7 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="40" t="s">
         <v>82</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1420,7 +1423,7 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="40" t="s">
         <v>84</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1428,7 +1431,7 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="40" t="s">
         <v>85</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1436,7 +1439,7 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="40" t="s">
         <v>86</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1444,7 +1447,7 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="40" t="s">
         <v>195</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1452,7 +1455,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="36" t="s">
         <v>200</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1460,7 +1463,7 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="37" t="s">
+      <c r="A20" s="36" t="s">
         <v>199</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1468,7 +1471,7 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="40" t="s">
         <v>74</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1476,7 +1479,7 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="40" t="s">
         <v>75</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1484,7 +1487,7 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="41" t="s">
+      <c r="A23" s="40" t="s">
         <v>76</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1492,7 +1495,7 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="41" t="s">
+      <c r="A24" s="40" t="s">
         <v>73</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1500,7 +1503,7 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="41" t="s">
+      <c r="A25" s="40" t="s">
         <v>95</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1508,7 +1511,7 @@
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="40" t="s">
         <v>98</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1516,7 +1519,7 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="41" t="s">
+      <c r="A27" s="40" t="s">
         <v>101</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1524,7 +1527,7 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="42" t="s">
         <v>192</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1532,7 +1535,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="42" t="s">
         <v>173</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1540,7 +1543,7 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="43" t="s">
+      <c r="A30" s="42" t="s">
         <v>165</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1548,7 +1551,7 @@
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="41" t="s">
         <v>191</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1556,7 +1559,7 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="40" t="s">
         <v>166</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1564,7 +1567,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="45" t="s">
+      <c r="A33" s="44" t="s">
         <v>104</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1572,7 +1575,7 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="45" t="s">
+      <c r="A34" s="44" t="s">
         <v>107</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1580,7 +1583,7 @@
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="45" t="s">
+      <c r="A35" s="44" t="s">
         <v>108</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1588,7 +1591,7 @@
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="44" t="s">
         <v>110</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -1596,7 +1599,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="28.8">
-      <c r="A37" s="45" t="s">
+      <c r="A37" s="44" t="s">
         <v>111</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1604,7 +1607,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="28.8">
-      <c r="A38" s="45" t="s">
+      <c r="A38" s="44" t="s">
         <v>112</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1612,7 +1615,7 @@
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="45" t="s">
+      <c r="A39" s="44" t="s">
         <v>113</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1620,7 +1623,7 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="41" t="s">
+      <c r="A40" s="40" t="s">
         <v>190</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1628,7 +1631,7 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="46" t="s">
+      <c r="A41" s="45" t="s">
         <v>186</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -1636,7 +1639,7 @@
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="47" t="s">
+      <c r="A42" s="46" t="s">
         <v>193</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1644,7 +1647,7 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="37" t="s">
+      <c r="A43" s="36" t="s">
         <v>202</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -1662,7 +1665,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1707,7 +1710,7 @@
       <c r="I1" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="38" t="s">
         <v>188</v>
       </c>
     </row>
@@ -1715,10 +1718,10 @@
       <c r="A2" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="B2" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="35" t="s">
+      <c r="B2" s="48" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="34" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="26" t="s">
@@ -1747,10 +1750,10 @@
       <c r="A3" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="35" t="s">
+      <c r="B3" s="48" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" s="34" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
@@ -1779,10 +1782,10 @@
       <c r="A4" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="B4" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="35" t="s">
+      <c r="B4" s="48" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" s="34" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
@@ -1797,10 +1800,10 @@
       <c r="G4" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="35" t="s">
         <v>174</v>
       </c>
       <c r="J4" t="s">
@@ -1811,10 +1814,10 @@
       <c r="A5" t="s">
         <v>166</v>
       </c>
-      <c r="B5" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="35" t="s">
+      <c r="B5" s="48" t="s">
+        <v>227</v>
+      </c>
+      <c r="C5" s="34" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
@@ -1840,11 +1843,11 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="B6" t="s">
-        <v>1</v>
+      <c r="B6" s="4" t="s">
+        <v>226</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -1877,12 +1880,14 @@
     <hyperlink ref="C3" r:id="rId2" xr:uid="{21C9AD85-C872-4CFF-8577-F0A32F2839F9}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{7711EFFC-8F92-405B-AC1B-008AFA2E71EB}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{2DAEEDB2-7E3F-429B-B695-7AB994FE65C5}"/>
-    <hyperlink ref="B5" r:id="rId5" xr:uid="{36238B94-2CA7-4241-A3FD-AC3F221FD5D6}"/>
-    <hyperlink ref="B3" r:id="rId6" xr:uid="{8CFB7073-8E2E-4C9D-8177-4DB6C87B24EC}"/>
-    <hyperlink ref="B4" r:id="rId7" xr:uid="{C25AB8EF-B12A-4BA5-8832-FBF9014647B6}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{C25AB8EF-B12A-4BA5-8832-FBF9014647B6}"/>
+    <hyperlink ref="B2" r:id="rId6" xr:uid="{15BF690C-72A2-46CA-848F-E93230300983}"/>
+    <hyperlink ref="B3" r:id="rId7" xr:uid="{B4F18C0A-0A79-4EB0-8467-E92089F81910}"/>
+    <hyperlink ref="B6" r:id="rId8" xr:uid="{4117839D-6D8C-4F86-89DC-3C2F9978433F}"/>
+    <hyperlink ref="B5" r:id="rId9" xr:uid="{6B1ED3D6-71F6-42DE-B23E-0E75250E3FAC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -1891,7 +1896,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1951,7 +1956,7 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="36" t="s">
         <v>202</v>
       </c>
       <c r="B2" t="s">
@@ -2001,8 +2006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D46A24-3205-4CDB-80C0-67C7443BF381}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2087,10 +2092,10 @@
       </c>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>226</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -2144,7 +2149,7 @@
       <c r="A3" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B3" s="49" t="s">
         <v>226</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -2158,7 +2163,7 @@
       <c r="A4" t="s">
         <v>185</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="49" t="s">
         <v>226</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -2214,7 +2219,7 @@
       <c r="A5" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="49" t="s">
         <v>226</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -2273,7 +2278,7 @@
       <c r="A6" t="s">
         <v>190</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B6" s="49" t="s">
         <v>226</v>
       </c>
       <c r="C6" t="s">
@@ -2326,7 +2331,7 @@
       <c r="A7" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="49" t="s">
         <v>226</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -2398,7 +2403,7 @@
   <dimension ref="A1:AD8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3006,8 +3011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77821D73-03CE-4B19-A8A0-8DB2062EDEA4}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3095,7 +3100,7 @@
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="36" t="s">
         <v>200</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -3137,7 +3142,7 @@
       <c r="N2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="48" t="s">
+      <c r="O2" s="47" t="s">
         <v>197</v>
       </c>
       <c r="P2" t="s">
@@ -3157,7 +3162,7 @@
       </c>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="36" t="s">
         <v>199</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -3199,7 +3204,7 @@
       <c r="N3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="48" t="s">
+      <c r="O3" s="47" t="s">
         <v>198</v>
       </c>
       <c r="P3" t="s">
@@ -3350,8 +3355,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC50B798-C00F-4686-80C0-D4DC574A8857}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3381,7 +3386,7 @@
         <v>74</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>1</v>
+        <v>228</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -3409,7 +3414,7 @@
         <v>76</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1</v>
+        <v>228</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -3423,7 +3428,7 @@
         <v>73</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1</v>
+        <v>228</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -3543,7 +3548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C9AF72F-B6B5-4632-88BA-4676BBA9E02D}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
27 scripts are executed
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaiVamshi.Kotla.SSTECH\PLSIBaseFramework\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817142F6-8EA1-4146-B7BF-9ACE9FC92CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B01625-BA9B-45C2-B347-4C2BBBBF785A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
@@ -728,7 +728,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -771,11 +771,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF6A8759"/>
-      <name val="Arial Unicode MS"/>
     </font>
     <font>
       <sz val="10"/>
@@ -918,7 +913,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -930,19 +925,16 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -960,8 +952,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -971,39 +963,39 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1317,7 +1309,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="38" t="s">
         <v>158</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1326,7 +1318,7 @@
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="38" t="s">
         <v>161</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1335,7 +1327,7 @@
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="39" t="s">
         <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1343,7 +1335,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="39" t="s">
         <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1351,7 +1343,7 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="39" t="s">
         <v>65</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -1359,7 +1351,7 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="38" t="s">
         <v>162</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1367,7 +1359,7 @@
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="40" t="s">
         <v>184</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1375,7 +1367,7 @@
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="39" t="s">
         <v>92</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1383,7 +1375,7 @@
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="40" t="s">
         <v>185</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1391,7 +1383,7 @@
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="41" t="s">
         <v>128</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1399,7 +1391,7 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="39" t="s">
         <v>78</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1407,7 +1399,7 @@
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="42" t="s">
         <v>81</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1415,7 +1407,7 @@
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="39" t="s">
         <v>82</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1423,7 +1415,7 @@
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="39" t="s">
         <v>84</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1431,7 +1423,7 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="39" t="s">
         <v>85</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1439,7 +1431,7 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="39" t="s">
         <v>86</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1447,7 +1439,7 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="39" t="s">
         <v>195</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1455,7 +1447,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>200</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1463,7 +1455,7 @@
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="35" t="s">
         <v>199</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1471,7 +1463,7 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="39" t="s">
         <v>74</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1479,7 +1471,7 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="39" t="s">
         <v>75</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1487,7 +1479,7 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>76</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1495,7 +1487,7 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="39" t="s">
         <v>73</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1503,7 +1495,7 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="39" t="s">
         <v>95</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1511,7 +1503,7 @@
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="40" t="s">
+      <c r="A26" s="39" t="s">
         <v>98</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1519,7 +1511,7 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="40" t="s">
+      <c r="A27" s="39" t="s">
         <v>101</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1527,7 +1519,7 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="41" t="s">
         <v>192</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1535,7 +1527,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="41" t="s">
         <v>173</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1543,7 +1535,7 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="41" t="s">
         <v>165</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1551,7 +1543,7 @@
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="40" t="s">
         <v>191</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1559,7 +1551,7 @@
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="40" t="s">
+      <c r="A32" s="39" t="s">
         <v>166</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1567,7 +1559,7 @@
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="44" t="s">
+      <c r="A33" s="43" t="s">
         <v>104</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1575,7 +1567,7 @@
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="43" t="s">
         <v>107</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1583,7 +1575,7 @@
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="43" t="s">
         <v>108</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1591,7 +1583,7 @@
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="43" t="s">
         <v>110</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -1599,7 +1591,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="28.8">
-      <c r="A37" s="44" t="s">
+      <c r="A37" s="43" t="s">
         <v>111</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1607,7 +1599,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="28.8">
-      <c r="A38" s="44" t="s">
+      <c r="A38" s="43" t="s">
         <v>112</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1615,7 +1607,7 @@
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="43" t="s">
         <v>113</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1623,7 +1615,7 @@
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="40" t="s">
+      <c r="A40" s="39" t="s">
         <v>190</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1631,7 +1623,7 @@
       </c>
     </row>
     <row r="41" spans="1:2">
-      <c r="A41" s="45" t="s">
+      <c r="A41" s="44" t="s">
         <v>186</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -1639,7 +1631,7 @@
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="46" t="s">
+      <c r="A42" s="45" t="s">
         <v>193</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1647,7 +1639,7 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="36" t="s">
+      <c r="A43" s="35" t="s">
         <v>202</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -1665,7 +1657,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1683,54 +1675,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>168</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="37" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>192</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="47" t="s">
         <v>226</v>
       </c>
-      <c r="C2" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="26" t="s">
+      <c r="C2" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>172</v>
       </c>
       <c r="G2" t="s">
@@ -1747,13 +1739,13 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="47" t="s">
         <v>226</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
@@ -1779,13 +1771,13 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="47" t="s">
         <v>227</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
@@ -1797,13 +1789,13 @@
       <c r="F4" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="35" t="s">
+      <c r="H4" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="34" t="s">
         <v>174</v>
       </c>
       <c r="J4" t="s">
@@ -1814,10 +1806,10 @@
       <c r="A5" t="s">
         <v>166</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="47" t="s">
         <v>227</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="33" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
@@ -1843,7 +1835,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="35" t="s">
         <v>191</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1956,7 +1948,7 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>202</v>
       </c>
       <c r="B2" t="s">
@@ -1980,10 +1972,10 @@
       <c r="H2" t="s">
         <v>221</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="20" t="s">
         <v>217</v>
       </c>
       <c r="K2" t="s">
@@ -1992,7 +1984,7 @@
       <c r="L2" t="s">
         <v>219</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="20" t="s">
         <v>215</v>
       </c>
     </row>
@@ -2007,7 +1999,7 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2033,7 +2025,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="6" customFormat="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>60</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -2069,22 +2061,22 @@
       <c r="L1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="22" t="s">
+      <c r="O1" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="P1" s="22" t="s">
+      <c r="P1" s="21" t="s">
         <v>27</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="R1" s="22" t="s">
         <v>119</v>
       </c>
       <c r="S1" s="6" t="s">
@@ -2092,50 +2084,50 @@
       </c>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>226</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="O2" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="P2" s="26" t="s">
+      <c r="P2" s="25" t="s">
         <v>71</v>
       </c>
       <c r="Q2" t="s">
@@ -2149,7 +2141,7 @@
       <c r="A3" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>226</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -2163,7 +2155,7 @@
       <c r="A4" t="s">
         <v>185</v>
       </c>
-      <c r="B4" s="49" t="s">
+      <c r="B4" s="48" t="s">
         <v>226</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -2172,40 +2164,40 @@
       <c r="D4" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="I4" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="O4" s="25" t="s">
+      <c r="O4" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="P4" s="26" t="s">
+      <c r="P4" s="25" t="s">
         <v>71</v>
       </c>
       <c r="Q4" t="s">
@@ -2216,10 +2208,10 @@
       </c>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="48" t="s">
         <v>226</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -2231,10 +2223,10 @@
       <c r="E5" t="s">
         <v>129</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="25" t="s">
         <v>131</v>
       </c>
       <c r="H5" t="s">
@@ -2278,7 +2270,7 @@
       <c r="A6" t="s">
         <v>190</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="48" t="s">
         <v>226</v>
       </c>
       <c r="C6" t="s">
@@ -2328,10 +2320,10 @@
       </c>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>193</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="48" t="s">
         <v>226</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -2340,40 +2332,40 @@
       <c r="D7" t="s">
         <v>129</v>
       </c>
-      <c r="E7" s="26" t="s">
-        <v>129</v>
-      </c>
-      <c r="F7" s="26" t="s">
+      <c r="E7" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="25" t="s">
+      <c r="J7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="25" t="s">
+      <c r="K7" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="25" t="s">
+      <c r="L7" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="25" t="s">
+      <c r="M7" s="24" t="s">
         <v>194</v>
       </c>
-      <c r="N7" s="25" t="s">
+      <c r="N7" s="24" t="s">
         <v>224</v>
       </c>
-      <c r="O7" s="25" t="s">
+      <c r="O7" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="P7" s="26" t="s">
+      <c r="P7" s="25" t="s">
         <v>71</v>
       </c>
       <c r="Q7" t="s">
@@ -2403,7 +2395,7 @@
   <dimension ref="A1:AD8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2449,233 +2441,233 @@
       <c r="G1" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="Q1" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="R1" s="27" t="s">
+      <c r="R1" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="S1" s="27" t="s">
+      <c r="S1" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="T1" s="27" t="s">
+      <c r="T1" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="U1" s="27" t="s">
+      <c r="U1" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="V1" s="27" t="s">
+      <c r="V1" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="W1" s="27" t="s">
+      <c r="W1" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="X1" s="27" t="s">
+      <c r="X1" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="Y1" s="27" t="s">
+      <c r="Y1" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="Z1" s="27" t="s">
+      <c r="Z1" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="AA1" s="27" t="s">
+      <c r="AA1" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="AB1" s="27" t="s">
+      <c r="AB1" s="26" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:30">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="28">
+        <v>0.73749999999999993</v>
+      </c>
+      <c r="E2" s="28">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="F2" s="29">
+        <v>2.65</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="H2" s="31">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="29">
+      <c r="I2" s="31">
+        <v>1</v>
+      </c>
+      <c r="J2" s="31">
+        <v>170</v>
+      </c>
+      <c r="K2" s="31">
+        <v>2</v>
+      </c>
+      <c r="L2" s="31">
+        <v>2</v>
+      </c>
+      <c r="M2" s="31">
+        <v>1</v>
+      </c>
+      <c r="N2" s="31">
+        <v>60</v>
+      </c>
+      <c r="O2" s="31">
+        <v>5</v>
+      </c>
+      <c r="P2" s="31">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="31">
+        <v>3</v>
+      </c>
+      <c r="R2" s="31">
+        <v>20</v>
+      </c>
+      <c r="S2" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="T2" s="31">
+        <v>1.25</v>
+      </c>
+      <c r="U2" s="31">
+        <v>1.5</v>
+      </c>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="31">
+        <v>7</v>
+      </c>
+      <c r="Y2" s="31">
+        <v>3</v>
+      </c>
+      <c r="Z2" s="31">
+        <v>40</v>
+      </c>
+      <c r="AA2" s="31">
+        <v>5</v>
+      </c>
+      <c r="AB2" s="31">
+        <v>120</v>
+      </c>
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30"/>
+    </row>
+    <row r="3" spans="1:30">
+      <c r="A3" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="28">
         <v>0.73749999999999993</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E3" s="28">
         <v>0.78472222222222221</v>
       </c>
-      <c r="F2" s="30">
+      <c r="F3" s="29">
         <v>2.65</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G3" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="H2" s="32">
+      <c r="H3" s="31">
         <v>1</v>
       </c>
-      <c r="I2" s="32">
+      <c r="I3" s="31">
         <v>1</v>
       </c>
-      <c r="J2" s="32">
+      <c r="J3" s="31">
         <v>170</v>
       </c>
-      <c r="K2" s="32">
-        <v>2</v>
-      </c>
-      <c r="L2" s="32">
-        <v>2</v>
-      </c>
-      <c r="M2" s="32">
+      <c r="K3" s="31">
+        <v>2</v>
+      </c>
+      <c r="L3" s="31">
+        <v>2</v>
+      </c>
+      <c r="M3" s="31">
         <v>1</v>
       </c>
-      <c r="N2" s="32">
+      <c r="N3" s="31">
         <v>60</v>
       </c>
-      <c r="O2" s="32">
+      <c r="O3" s="31">
         <v>5</v>
       </c>
-      <c r="P2" s="32">
+      <c r="P3" s="31">
         <v>4</v>
       </c>
-      <c r="Q2" s="32">
+      <c r="Q3" s="31">
         <v>3</v>
       </c>
-      <c r="R2" s="32">
+      <c r="R3" s="31">
         <v>20</v>
       </c>
-      <c r="S2" s="33" t="s">
+      <c r="S3" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="T2" s="32">
+      <c r="T3" s="31">
         <v>1.25</v>
       </c>
-      <c r="U2" s="32">
+      <c r="U3" s="31">
         <v>1.5</v>
       </c>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="32">
+      <c r="V3" s="32"/>
+      <c r="W3" s="32"/>
+      <c r="X3" s="31">
         <v>7</v>
       </c>
-      <c r="Y2" s="32">
+      <c r="Y3" s="31">
         <v>3</v>
       </c>
-      <c r="Z2" s="32">
+      <c r="Z3" s="31">
         <v>40</v>
       </c>
-      <c r="AA2" s="32">
+      <c r="AA3" s="31">
         <v>5</v>
       </c>
-      <c r="AB2" s="32">
-        <v>120</v>
-      </c>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-    </row>
-    <row r="3" spans="1:30">
-      <c r="A3" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="29">
-        <v>0.73749999999999993</v>
-      </c>
-      <c r="E3" s="29">
-        <v>0.78472222222222221</v>
-      </c>
-      <c r="F3" s="30">
-        <v>2.65</v>
-      </c>
-      <c r="G3" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="H3" s="32">
-        <v>1</v>
-      </c>
-      <c r="I3" s="32">
-        <v>1</v>
-      </c>
-      <c r="J3" s="32">
-        <v>170</v>
-      </c>
-      <c r="K3" s="32">
-        <v>2</v>
-      </c>
-      <c r="L3" s="32">
-        <v>2</v>
-      </c>
-      <c r="M3" s="32">
-        <v>1</v>
-      </c>
-      <c r="N3" s="32">
-        <v>60</v>
-      </c>
-      <c r="O3" s="32">
-        <v>5</v>
-      </c>
-      <c r="P3" s="32">
-        <v>4</v>
-      </c>
-      <c r="Q3" s="32">
-        <v>3</v>
-      </c>
-      <c r="R3" s="32">
-        <v>20</v>
-      </c>
-      <c r="S3" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="T3" s="32">
-        <v>1.25</v>
-      </c>
-      <c r="U3" s="32">
-        <v>1.5</v>
-      </c>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
-      <c r="X3" s="32">
-        <v>7</v>
-      </c>
-      <c r="Y3" s="32">
-        <v>3</v>
-      </c>
-      <c r="Z3" s="32">
-        <v>40</v>
-      </c>
-      <c r="AA3" s="32">
-        <v>5</v>
-      </c>
-      <c r="AB3" s="32">
+      <c r="AB3" s="31">
         <v>120</v>
       </c>
       <c r="AC3" s="7"/>
@@ -2685,8 +2677,8 @@
       <c r="A4" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>1</v>
+      <c r="B4" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
@@ -2696,8 +2688,8 @@
       <c r="A5" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>1</v>
+      <c r="B5" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>2</v>
@@ -2707,19 +2699,19 @@
       <c r="A6" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>1</v>
+      <c r="B6" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:30">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>1</v>
+      <c r="B7" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>2</v>
@@ -2729,11 +2721,11 @@
       </c>
     </row>
     <row r="8" spans="1:30">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>1</v>
+      <c r="B8" s="47" t="s">
+        <v>225</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>2</v>
@@ -2748,9 +2740,13 @@
     <hyperlink ref="C3" r:id="rId5" xr:uid="{3FD6D116-216A-4423-835A-F97000FF95CC}"/>
     <hyperlink ref="C7" r:id="rId6" xr:uid="{E7BB4DFE-A00A-494B-B573-2FA848FA84CF}"/>
     <hyperlink ref="C8" r:id="rId7" xr:uid="{AADD8828-4D21-4908-9221-0DCFA4071DA4}"/>
+    <hyperlink ref="B2" r:id="rId8" xr:uid="{702090F1-D65E-4B43-8116-49D16CD7A344}"/>
+    <hyperlink ref="B4" r:id="rId9" xr:uid="{19B58D5C-E0A0-4C0E-8D70-E2D8E7A9F58E}"/>
+    <hyperlink ref="B5:B7" r:id="rId10" display="gangadhar.m@sstech.us" xr:uid="{656BAC6F-28F9-4DC5-8F87-75919D119C60}"/>
+    <hyperlink ref="B8" r:id="rId11" xr:uid="{7083E1D2-F435-446C-ACA8-690E33C58B84}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -2776,35 +2772,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
@@ -2816,7 +2812,7 @@
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>109</v>
       </c>
       <c r="E2" s="4" t="s">
@@ -2833,7 +2829,7 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>81</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2842,7 +2838,7 @@
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>109</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -2868,7 +2864,7 @@
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>109</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -2894,7 +2890,7 @@
       <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>109</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -2920,7 +2916,7 @@
       <c r="C6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>109</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -2949,7 +2945,7 @@
       <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>109</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -2992,7 +2988,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{0D458867-A002-45E1-B365-545961492A16}"/>
     <hyperlink ref="E3:E7" r:id="rId2" display="deepa.pattar@sstech.us" xr:uid="{61492ADE-3336-44E6-9318-42D2D7523F4D}"/>
@@ -3100,7 +3096,7 @@
       </c>
     </row>
     <row r="2" spans="1:20">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>200</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -3142,7 +3138,7 @@
       <c r="N2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="47" t="s">
+      <c r="O2" s="46" t="s">
         <v>197</v>
       </c>
       <c r="P2" t="s">
@@ -3162,7 +3158,7 @@
       </c>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="35" t="s">
         <v>199</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -3204,7 +3200,7 @@
       <c r="N3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="47" t="s">
+      <c r="O3" s="46" t="s">
         <v>198</v>
       </c>
       <c r="P3" t="s">
@@ -3242,7 +3238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB21362-C935-4D70-8A2D-2CFAFF7C4674}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
@@ -3355,7 +3351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC50B798-C00F-4686-80C0-D4DC574A8857}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -3368,16 +3364,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>188</v>
       </c>
     </row>
@@ -3391,7 +3387,7 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3405,7 +3401,7 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3419,7 +3415,7 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3453,8 +3449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C956B14F-0A4B-4BD7-A86C-D911C2214633}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3476,61 +3472,61 @@
       <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>1</v>
+      <c r="B2" s="48" t="s">
+        <v>226</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>1</v>
+      <c r="B3" s="48" t="s">
+        <v>226</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>1</v>
+      <c r="B4" s="48" t="s">
+        <v>226</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3539,6 +3535,8 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{D9097781-0FAD-493C-9670-CEA54F22237C}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{048F86AF-02A7-43B2-9117-5783D566A05C}"/>
     <hyperlink ref="C4" r:id="rId3" xr:uid="{42365D77-69E6-4644-A553-C7BF1E28C142}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{9255B575-F868-46AC-A994-F6C2E6BD1D30}"/>
+    <hyperlink ref="B3:B4" r:id="rId5" display="sravani.bandaru@sstech.us" xr:uid="{9A70ECE9-620A-480D-BEB1-C52794BEB28E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3549,7 +3547,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3564,37 +3562,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
+      <c r="B2" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -3605,16 +3603,16 @@
       <c r="E2" t="s">
         <v>105</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
+      <c r="B3" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -3627,11 +3625,11 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="B4" t="s">
-        <v>1</v>
+      <c r="B4" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -3644,11 +3642,11 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="B5" t="s">
-        <v>1</v>
+      <c r="B5" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -3661,16 +3659,16 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="B6" t="s">
-        <v>1</v>
+      <c r="B6" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="18" t="s">
         <v>109</v>
       </c>
       <c r="E6" t="s">
@@ -3678,11 +3676,11 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="B7" t="s">
-        <v>1</v>
+      <c r="B7" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -3695,11 +3693,11 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="B8" t="s">
-        <v>1</v>
+      <c r="B8" s="47" t="s">
+        <v>226</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>2</v>
@@ -3718,14 +3716,15 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="19"/>
+      <c r="A9" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C12" r:id="rId1" display="Welcome@1" xr:uid="{8F3E35E5-FF30-420A-BFB6-FDD10921CC00}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{B3C73D34-948D-4F1D-8BAC-27F416656071}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{A32E531E-3F0E-4487-9740-6966412A252F}"/>
-    <hyperlink ref="C8" r:id="rId4" xr:uid="{8F3E35E5-FF30-420A-BFB6-FDD10921CC00}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{A32E531E-3F0E-4487-9740-6966412A252F}"/>
+    <hyperlink ref="C8" r:id="rId3" xr:uid="{8F3E35E5-FF30-420A-BFB6-FDD10921CC00}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{D0354CD3-973B-4571-A569-36FB285BD704}"/>
+    <hyperlink ref="B3:B8" r:id="rId5" display="sravani.bandaru@sstech.us" xr:uid="{FA92DD12-C0DD-4D29-BB7C-89104C0625E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changes done in the TestNG.xml file for 4th time
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaiVamshi.Kotla.SSTECH\PLSIBaseFramework\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B01625-BA9B-45C2-B347-4C2BBBBF785A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5F132A-2BF0-4B3C-B3D9-DD419ADAB2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3450,7 +3450,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Changes made for FinancePayout and InterpreAptTabs Test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaiVamshi.Kotla.SSTECH\PLSIBaseFramework\PLSIAutomationBase\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Working _PLSI_current_ Automattion\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5F132A-2BF0-4B3C-B3D9-DD419ADAB2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9A483B-D6AE-406B-B26C-812220854E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
@@ -2394,8 +2394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D31F42-B4A6-433A-86B0-A7DD37BBCE9B}">
   <dimension ref="A1:AD8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" activeCellId="1" sqref="B3 C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2510,7 +2510,7 @@
         <v>158</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>226</v>
+        <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
@@ -2594,7 +2594,7 @@
         <v>161</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>226</v>
+        <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
@@ -3449,7 +3449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C956B14F-0A4B-4BD7-A86C-D911C2214633}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
change in AppRejectAcceptToFinalize_Test.java, DashBoardPage.java, InterpreterDashboardPage.java, PLSI_Automation_Data.xlsx.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PLSI_Automation_Data.xlsx
+++ b/src/test/resources/data/PLSI_Automation_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Working _PLSI_current_ Automattion\PLSIAutomationBase\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A841A1BA-6A9C-4397-9036-816E448C00F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB5514C-F391-461F-B67C-F8D001F70E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="229">
   <si>
     <t>Password</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Fitness</t>
   </si>
   <si>
-    <t>Abramson Building</t>
-  </si>
-  <si>
     <t>Department</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
     <t>14:56PM</t>
   </si>
   <si>
-    <t>CSE</t>
-  </si>
-  <si>
     <t>Pavan</t>
   </si>
   <si>
@@ -646,9 +640,6 @@
     <t>addRequesterforClient</t>
   </si>
   <si>
-    <t>Healthcare</t>
-  </si>
-  <si>
     <t>ClientDetails</t>
   </si>
   <si>
@@ -728,6 +719,9 @@
   </si>
   <si>
     <t>CS</t>
+  </si>
+  <si>
+    <t>PLSI</t>
   </si>
 </sst>
 </file>
@@ -1308,348 +1302,348 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="38" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="38" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="39" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="39" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="38" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="40" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="39" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="40" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="41" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="39" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="39" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="39" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="35" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="39" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="39" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="39" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="39" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="39" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="39" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="41" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="41" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="41" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="40" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="39" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="43" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="43" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="28.8">
       <c r="A37" s="43" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="28.8">
       <c r="A38" s="43" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="43" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="39" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="44" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="45" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="35" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -1682,194 +1676,194 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>62</v>
       </c>
       <c r="C1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="E1" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>169</v>
-      </c>
       <c r="G1" s="23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H1" s="23" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I1" s="23" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J1" s="37" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="24" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C2" s="33" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="E2" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="E2" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>172</v>
-      </c>
       <c r="G2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H4" s="34" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="I4" s="34" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C5" s="33" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="35" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -1893,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F3517F0-85DC-46BC-AE96-D76A2E9F5DE3}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1914,48 +1908,48 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>211</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="35" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1964,34 +1958,34 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>203</v>
+        <v>228</v>
       </c>
       <c r="E2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="I2" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="K2" t="s">
+        <v>215</v>
+      </c>
+      <c r="L2" t="s">
         <v>216</v>
       </c>
-      <c r="J2" s="20" t="s">
-        <v>217</v>
-      </c>
-      <c r="K2" t="s">
-        <v>218</v>
-      </c>
-      <c r="L2" t="s">
-        <v>219</v>
-      </c>
       <c r="M2" s="20" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2004,8 +1998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D46A24-3205-4CDB-80C0-67C7443BF381}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6:L7"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2032,16 +2026,16 @@
   <sheetData>
     <row r="1" spans="1:19" s="6" customFormat="1">
       <c r="A1" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -2065,49 +2059,49 @@
         <v>9</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M1" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="O1" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="21" t="s">
         <v>26</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="P1" s="21" t="s">
-        <v>27</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>10</v>
       </c>
       <c r="R1" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="36" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>226</v>
+        <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>11</v>
@@ -2119,65 +2113,65 @@
         <v>13</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="M2" s="24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N2" s="24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O2" s="24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P2" s="25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" s="48" t="s">
-        <v>226</v>
+        <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>226</v>
+        <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H4" s="24" t="s">
         <v>11</v>
@@ -2189,110 +2183,110 @@
         <v>13</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="M4" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="N4" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="O4" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="N4" s="24" t="s">
+      <c r="P4" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>77</v>
+      </c>
+      <c r="R4" t="s">
         <v>125</v>
-      </c>
-      <c r="O4" s="24" t="s">
-        <v>126</v>
-      </c>
-      <c r="P4" s="25" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>79</v>
-      </c>
-      <c r="R4" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="48" t="s">
-        <v>226</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="G5" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="E5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F5" s="25" t="s">
+      <c r="H5" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" t="s">
+        <v>127</v>
+      </c>
+      <c r="J5" t="s">
+        <v>127</v>
+      </c>
+      <c r="K5" t="s">
+        <v>127</v>
+      </c>
+      <c r="L5" t="s">
+        <v>127</v>
+      </c>
+      <c r="M5" t="s">
+        <v>127</v>
+      </c>
+      <c r="N5" t="s">
+        <v>127</v>
+      </c>
+      <c r="O5" t="s">
+        <v>127</v>
+      </c>
+      <c r="P5" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>127</v>
+      </c>
+      <c r="R5" t="s">
+        <v>127</v>
+      </c>
+      <c r="S5" t="s">
         <v>130</v>
-      </c>
-      <c r="G5" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="H5" t="s">
-        <v>129</v>
-      </c>
-      <c r="I5" t="s">
-        <v>129</v>
-      </c>
-      <c r="J5" t="s">
-        <v>129</v>
-      </c>
-      <c r="K5" t="s">
-        <v>129</v>
-      </c>
-      <c r="L5" t="s">
-        <v>129</v>
-      </c>
-      <c r="M5" t="s">
-        <v>129</v>
-      </c>
-      <c r="N5" t="s">
-        <v>129</v>
-      </c>
-      <c r="O5" t="s">
-        <v>129</v>
-      </c>
-      <c r="P5" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>129</v>
-      </c>
-      <c r="R5" t="s">
-        <v>129</v>
-      </c>
-      <c r="S5" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>226</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E6" s="5">
         <v>44965</v>
       </c>
       <c r="F6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H6" t="s">
         <v>11</v>
@@ -2304,48 +2298,48 @@
         <v>13</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L6" s="24" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="M6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P6" s="5">
         <v>35803</v>
       </c>
       <c r="Q6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="16" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>226</v>
+        <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H7" s="24" t="s">
         <v>11</v>
@@ -2357,28 +2351,28 @@
         <v>13</v>
       </c>
       <c r="K7" s="24" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L7" s="24" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="M7" s="24" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="N7" s="24" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="O7" s="24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P7" s="25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="Q7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -2389,10 +2383,14 @@
     <hyperlink ref="C5" r:id="rId4" xr:uid="{A19147BA-3A11-43A7-99EA-1DADEB7FAC25}"/>
     <hyperlink ref="C7" r:id="rId5" xr:uid="{D5D17004-3FC0-4EA0-98DC-166C1EB3FCE4}"/>
     <hyperlink ref="B2" r:id="rId6" xr:uid="{B7145825-7747-4E7F-882E-DC2FFB5E3E1F}"/>
-    <hyperlink ref="B3:B7" r:id="rId7" display="sravani.bandaru@sstech.us" xr:uid="{D85EA05C-8D3F-4BDF-8BAC-7AC8A1C3A7EC}"/>
+    <hyperlink ref="B3" r:id="rId7" xr:uid="{42CB472B-8059-4D23-BE18-58FF4A9833F4}"/>
+    <hyperlink ref="B4" r:id="rId8" xr:uid="{A0A4780B-DC25-43C0-8FFC-C538FA662ABC}"/>
+    <hyperlink ref="B5" r:id="rId9" xr:uid="{D79204EA-D995-434E-8314-1AF41F54B603}"/>
+    <hyperlink ref="B6" r:id="rId10" xr:uid="{212DC4E6-DB01-411E-A32B-91813FD8D0B2}"/>
+    <hyperlink ref="B7" r:id="rId11" xr:uid="{28DBD8F8-6CA0-4243-8E21-746B07BDD7BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -2427,93 +2425,93 @@
   <sheetData>
     <row r="1" spans="1:30">
       <c r="A1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="I1" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="J1" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="L1" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="M1" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="N1" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="O1" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="P1" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="Q1" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="R1" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="S1" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="T1" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="S1" s="26" t="s">
+      <c r="U1" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="T1" s="26" t="s">
+      <c r="V1" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="U1" s="26" t="s">
+      <c r="W1" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="V1" s="26" t="s">
+      <c r="X1" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="W1" s="26" t="s">
+      <c r="Y1" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="X1" s="26" t="s">
+      <c r="Z1" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="Y1" s="26" t="s">
+      <c r="AA1" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="Z1" s="26" t="s">
+      <c r="AB1" s="26" t="s">
         <v>155</v>
-      </c>
-      <c r="AA1" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="AB1" s="26" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>1</v>
@@ -2531,7 +2529,7 @@
         <v>2.65</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H2" s="31">
         <v>1</v>
@@ -2567,7 +2565,7 @@
         <v>20</v>
       </c>
       <c r="S2" s="32" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="T2" s="31">
         <v>1.25</v>
@@ -2597,7 +2595,7 @@
     </row>
     <row r="3" spans="1:30">
       <c r="A3" s="27" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B3" s="47" t="s">
         <v>1</v>
@@ -2615,7 +2613,7 @@
         <v>2.65</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H3" s="31">
         <v>1</v>
@@ -2651,7 +2649,7 @@
         <v>20</v>
       </c>
       <c r="S3" s="32" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="T3" s="31">
         <v>1.25</v>
@@ -2681,10 +2679,10 @@
     </row>
     <row r="4" spans="1:30">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>2</v>
@@ -2692,10 +2690,10 @@
     </row>
     <row r="5" spans="1:30">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>2</v>
@@ -2703,10 +2701,10 @@
     </row>
     <row r="6" spans="1:30">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>2</v>
@@ -2714,24 +2712,24 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="27" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="27" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>2</v>
@@ -2761,7 +2759,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2772,6 +2770,7 @@
     <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
     <col min="6" max="6" width="24.44140625" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
     <col min="8" max="8" width="27.33203125" customWidth="1"/>
     <col min="9" max="9" width="20.88671875" customWidth="1"/>
     <col min="10" max="10" width="18.44140625" customWidth="1"/>
@@ -2779,38 +2778,38 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>18</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>19</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>10</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
@@ -2819,24 +2818,24 @@
         <v>2</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>1</v>
@@ -2845,24 +2844,24 @@
         <v>2</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>1</v>
@@ -2871,24 +2870,24 @@
         <v>2</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>1</v>
@@ -2897,24 +2896,24 @@
         <v>2</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>1</v>
@@ -2923,74 +2922,74 @@
         <v>2</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>225</v>
+        <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -3014,7 +3013,7 @@
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3041,10 +3040,10 @@
   <sheetData>
     <row r="1" spans="1:20" s="8" customFormat="1">
       <c r="A1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>0</v>
@@ -3053,10 +3052,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>22</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>6</v>
@@ -3065,60 +3064,60 @@
         <v>7</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="Q1" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="R1" s="8" t="s">
         <v>10</v>
       </c>
       <c r="S1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="35" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
         <v>32</v>
-      </c>
-      <c r="F2" t="s">
-        <v>33</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -3127,60 +3126,60 @@
         <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>226</v>
       </c>
       <c r="K2" t="s">
+        <v>227</v>
+      </c>
+      <c r="L2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="O2" s="46" t="s">
+        <v>195</v>
+      </c>
+      <c r="P2" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="Q2" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S2" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" t="s">
         <v>38</v>
-      </c>
-      <c r="R2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2" t="s">
-        <v>39</v>
-      </c>
-      <c r="T2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
         <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -3189,40 +3188,40 @@
         <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>226</v>
       </c>
       <c r="K3" t="s">
+        <v>227</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="L3" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="O3" s="46" t="s">
+        <v>196</v>
+      </c>
+      <c r="P3" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="Q3" t="s">
         <v>36</v>
       </c>
-      <c r="O3" s="46" t="s">
-        <v>198</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3" t="s">
         <v>37</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="T3" t="s">
         <v>38</v>
-      </c>
-      <c r="R3" t="s">
-        <v>21</v>
-      </c>
-      <c r="S3" t="s">
-        <v>39</v>
-      </c>
-      <c r="T3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -3244,7 +3243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB21362-C935-4D70-8A2D-2CFAFF7C4674}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
@@ -3263,57 +3262,57 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>51</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
         <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" t="s">
-        <v>55</v>
       </c>
       <c r="E2">
         <v>8452</v>
@@ -3322,25 +3321,25 @@
         <v>9133221196</v>
       </c>
       <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="H2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="J2">
         <v>50081</v>
       </c>
       <c r="K2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -3371,66 +3370,66 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>62</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -3470,24 +3469,24 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B2" s="48" t="s">
         <v>1</v>
@@ -3496,15 +3495,15 @@
         <v>2</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B3" s="48" t="s">
         <v>1</v>
@@ -3513,15 +3512,15 @@
         <v>2</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B4" s="48" t="s">
         <v>1</v>
@@ -3530,10 +3529,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -3568,156 +3567,156 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>17</v>
-      </c>
       <c r="D1" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>116</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>223</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>104</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>226</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B4" s="47" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B5" s="47" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8">
       <c r="A6" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8">
       <c r="A7" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B7" s="47" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:8">

</xml_diff>